<commit_message>
Revert "adding term 2.0.0"
This reverts commit f11b7ba2b6e1439b29c966e38ff2fe443ac25ded.
</commit_message>
<xml_diff>
--- a/term/CodeSystem-CareSocialCodes.xlsx
+++ b/term/CodeSystem-CareSocialCodes.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="225">
   <si>
     <t>Property</t>
   </si>
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>2.0.0</t>
+    <t>1.1.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-06-01T22:25:19+02:00</t>
+    <t>2023-07-10T23:08:03+02:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -69,13 +69,13 @@
     <t>Contact</t>
   </si>
   <si>
-    <t>Kommunernes Landsforening (http://kl.dk)</t>
+    <t>No display for ContactDetail</t>
   </si>
   <si>
     <t>Description</t>
   </si>
   <si>
-    <t>Administrative/technical codes in Local Govenment Denmark (KL), associated with common use cases across areas or kl-core</t>
+    <t>Administrative/technical codes in Local Govenment Denmark (KL), associated with KLCommonCareSocial</t>
   </si>
   <si>
     <t>Purpose</t>
@@ -144,10 +144,10 @@
     <t>effe55c7-572c-4a99-8fb4-2a9dda2f6572</t>
   </si>
   <si>
-    <t>FFB st�ttebehovsvurdering</t>
-  </si>
-  <si>
-    <t>Angiver, hvor stort et behov borgeren har for hj�lp og st�tte.</t>
+    <t>FFB støttebehovsvurdering</t>
+  </si>
+  <si>
+    <t>Angiver, hvor stort et behov borgeren har for hjælp og støtte.</t>
   </si>
   <si>
     <t>053a301d-1bb8-4cc4-b781-87825ecf0ef8</t>
@@ -159,10 +159,19 @@
     <t>Vurdering der sammenholder oplysninger fra udredning mhp en samlet faglig analyse og konklusion.</t>
   </si>
   <si>
+    <t>54c4ffea-7caf-4edc-8aa9-ef6e0be26c4c</t>
+  </si>
+  <si>
+    <t>FSIII helhedsvurdering</t>
+  </si>
+  <si>
+    <t>Sagsvurdering, der sammenholder resultaterne af en myndighedsudredning og den øvrige sagsoplysning med henblik på at træffe en afgørelse</t>
+  </si>
+  <si>
     <t>3f7a8ca0-afca-4b0d-8773-a99b5f2f8aaf</t>
   </si>
   <si>
-    <t>VUM Borgerens perspektiv p� indsatsen</t>
+    <t>VUM Borgerens perspektiv på indsatsen</t>
   </si>
   <si>
     <t>f52887de-023f-4193-b6b0-4b0a37b1cffc</t>
@@ -171,21 +180,30 @@
     <t>VUM Borgerens ressourcer i forhold til indsatsen</t>
   </si>
   <si>
-    <t>54c4ffea-7caf-4edc-8aa9-ef6e0be26c4c</t>
-  </si>
-  <si>
-    <t>FSIII helhedsvurdering</t>
-  </si>
-  <si>
-    <t>Sagsvurdering, der sammenholder resultaterne af en myndighedsudredning og den �vrige sagsoplysning med henblik p� at tr�ffe en afg�relse</t>
-  </si>
-  <si>
     <t>7b41185e-eeb4-437d-8120-5d51bbd27a79</t>
   </si>
   <si>
     <t>Indsats/ydelses-anmodning</t>
   </si>
   <si>
+    <t>ad865929-7363-4b2d-a271-01993181fbaf</t>
+  </si>
+  <si>
+    <t>Hjemmepleje</t>
+  </si>
+  <si>
+    <t>Der anmodes om hjemmepleje</t>
+  </si>
+  <si>
+    <t>490ab7be-ddb1-4a54-baf1-009fe6e8a83b</t>
+  </si>
+  <si>
+    <t>Hjemmesygepleje</t>
+  </si>
+  <si>
+    <t>Der anmodes om sygepleje</t>
+  </si>
+  <si>
     <t>4a297733-4d66-4726-a933-590d55cf91e0</t>
   </si>
   <si>
@@ -195,49 +213,22 @@
     <t>Der anmodes om en social indsats</t>
   </si>
   <si>
-    <t>ad865929-7363-4b2d-a271-01993181fbaf</t>
-  </si>
-  <si>
-    <t>Kommunal pleje og omsorg</t>
-  </si>
-  <si>
-    <t>Der anmodes om kommunal pleje og omsorg fx hjemmepleje til �ldre borger.</t>
-  </si>
-  <si>
-    <t>490ab7be-ddb1-4a54-baf1-009fe6e8a83b</t>
-  </si>
-  <si>
-    <t>Kommunal sygepleje</t>
-  </si>
-  <si>
-    <t>Der anmodes om kommunal sygepleje.</t>
-  </si>
-  <si>
     <t>a71921ea-fe83-441d-933b-cc21d0b3c8c3</t>
   </si>
   <si>
-    <t>Kommunal Sundhedsfremme og forebyggelse</t>
-  </si>
-  <si>
-    <t>Der anmodes om kommunal sundhedsfremme og forebyggelse efter SUL �119.</t>
+    <t>Sundhedsfremme og forebyggelse</t>
+  </si>
+  <si>
+    <t>Der anmodes om sundhedsfremme og forebyggelse</t>
   </si>
   <si>
     <t>7fc66c15-0cb3-4c89-9e18-f3a01e6a6592</t>
   </si>
   <si>
-    <t>Kommunal genoptr�ning efter sygehusophold</t>
-  </si>
-  <si>
-    <t>Der anmodes om kommunal genoptr�ning efter sygehusophold efter SUL �140.</t>
-  </si>
-  <si>
-    <t>d267ac44-8d7f-43e9-8535-ab3da350649f</t>
-  </si>
-  <si>
-    <t>Kommunalt hj�lpemiddelomr�de</t>
-  </si>
-  <si>
-    <t>Der anmodes om hj�lpemidler og lignende, der ligger indenfor det kommunale hj�lpemiddelomr�de dvs � 112, � 113, � 114, � 116 i Serviceloven.</t>
+    <t>Træning</t>
+  </si>
+  <si>
+    <t>Der anmodes om træning</t>
   </si>
   <si>
     <t>b5731132-f6b9-4a47-995d-681d2b755d4f</t>
@@ -267,58 +258,13 @@
     <t>Sagsbehandler er kilde til oplysning eller vurdering</t>
   </si>
   <si>
-    <t>329774f9-7700-47cf-9c00-63765d9e8078</t>
-  </si>
-  <si>
-    <t>Medarbejder og p�r�rende alene</t>
-  </si>
-  <si>
-    <t>En medarbejder og p�r�rende er sammen, men uden input fra borger, kilde til oplysning eller vurdering. Fx PUF sp�rgeskema i sundhedsplejen.</t>
-  </si>
-  <si>
-    <t>8fe80acb-2c2a-4f10-b2b8-ddb77d2f69dc</t>
-  </si>
-  <si>
-    <t>Medarbejder alene</t>
-  </si>
-  <si>
-    <t>Medarbejderen er alene kilde til oplysning eller vurdering. Fx AIMS skema i sundhedsplejen.</t>
-  </si>
-  <si>
-    <t>12428e48-7df8-441f-9a89-d92bb7874066</t>
-  </si>
-  <si>
-    <t>Borger st�ttet af medarbejder</t>
-  </si>
-  <si>
-    <t>Borger fik hj�lp af en medarbejder til at komme med oplysninger eller vurderinger. Fx �ldre borger der f�r hj�lp til at udfylde WHO5 sp�rgeskema.</t>
-  </si>
-  <si>
-    <t>b66dc78a-a673-43fc-8ac0-1e859ba626e0</t>
-  </si>
-  <si>
-    <t>Borger st�ttet af p�r�rende</t>
-  </si>
-  <si>
-    <t>Borger fik hj�lp af en p�r�rende til at komme med oplysninger eller vurderinger. Fx �ldre borger der f�r hj�lp til at udfylde WHO5 sp�rgeskema.</t>
-  </si>
-  <si>
-    <t>166d2437-4e47-4a52-bd94-cdbe91086ca6</t>
-  </si>
-  <si>
-    <t>P�r�rende alene</t>
-  </si>
-  <si>
-    <t>P�r�rende er alene, uden input fra borger, kilde til oplysninger eller vuderderinger. Fx WHO 5 sp�rgeskema for sv�kket �ldre borger udfyldt af datter.</t>
-  </si>
-  <si>
     <t>63338442-7b2e-405b-acc0-142361ef19f1</t>
   </si>
   <si>
     <t>Andre</t>
   </si>
   <si>
-    <t>Andre end borger og sagsbehandler er kilde til oplysning eller vurdering. Fx l�ge, p�r�rende og udf�rer. Denne definition af andre, bruges kun p� voksensocialomr�det.</t>
+    <t>Andre end borger og sagsbehandler er kilde til oplysning eller vurdering. Fx læge, pårørende og udfører</t>
   </si>
   <si>
     <t>3</t>
@@ -327,10 +273,10 @@
     <t>f00a6844-1005-401d-965d-1c5859df7beb</t>
   </si>
   <si>
-    <t>Udf�rer</t>
-  </si>
-  <si>
-    <t>Udf�rer er kilde til oplysning eller vurdering</t>
+    <t>Udfører</t>
+  </si>
+  <si>
+    <t>Udfører er kilde til oplysning eller vurdering</t>
   </si>
   <si>
     <t>25303acd-dcaf-4a8e-a8a3-3961a43858aa</t>
@@ -354,10 +300,10 @@
     <t>9f03dfbb-7a97-45a5-94db-d4c3501714a9</t>
   </si>
   <si>
-    <t>opf�lgning</t>
-  </si>
-  <si>
-    <t>opf�lgning foretaget ved kontakt</t>
+    <t>opfølgning</t>
+  </si>
+  <si>
+    <t>opfølgning foretaget ved kontakt</t>
   </si>
   <si>
     <t>829ac647-c7fc-4964-836b-f708d886e0e3</t>
@@ -372,28 +318,28 @@
     <t>15775b0a-7ec6-469e-9d3c-a81fbc9a1b45</t>
   </si>
   <si>
-    <t>udf�relse af akutindsats</t>
-  </si>
-  <si>
-    <t>Akutindsats, bevilget af l�ge eller akutteam, udf�rt ved kontakt</t>
+    <t>udførelse af akutindsats</t>
+  </si>
+  <si>
+    <t>Akutindsats, bevilget af læge eller akutteam, udført ved kontakt</t>
   </si>
   <si>
     <t>c03b426a-4348-407f-b343-f4baa9759c72</t>
   </si>
   <si>
-    <t>udf�relse af ikke-bevilget indsats</t>
-  </si>
-  <si>
-    <t>Indsats, der ikke i forvejen var bevilget, udf�rt ved kontakt</t>
+    <t>udførelse af ikke-bevilget indsats</t>
+  </si>
+  <si>
+    <t>Indsats, der ikke i forvejen var bevilget, udført ved kontakt</t>
   </si>
   <si>
     <t>784275f1-6822-4a88-b361-d958007d5253</t>
   </si>
   <si>
-    <t>udf�relse af planlagt indsats</t>
-  </si>
-  <si>
-    <t>Planlagt indsats udf�rt ved kontakt</t>
+    <t>udførelse af planlagt indsats</t>
+  </si>
+  <si>
+    <t>Planlagt indsats udført ved kontakt</t>
   </si>
   <si>
     <t>9269c9a2-8220-447b-a127-811275b41062</t>
@@ -408,82 +354,106 @@
     <t>3762dd32-4123-43a8-815d-ec40d3697652</t>
   </si>
   <si>
-    <t>indforst�else ifm henvendelse</t>
+    <t>indforståelse ifm henvendelse</t>
   </si>
   <si>
     <t>54aeeba6-6aa2-4165-a5a8-bbd6f2f3b1eb</t>
   </si>
   <si>
-    <t>ikke indforst�et</t>
-  </si>
-  <si>
-    <t>Borger ikke indforst�et med henvendelse</t>
+    <t>ikke indforstået</t>
+  </si>
+  <si>
+    <t>Borger ikke indforstået med henvendelse</t>
   </si>
   <si>
     <t>e67035da-9179-466b-99ad-ea86835d38c9</t>
   </si>
   <si>
-    <t>indforst�et</t>
-  </si>
-  <si>
-    <t>Borger indforst�et med henvendelse</t>
+    <t>indforstået</t>
+  </si>
+  <si>
+    <t>Borger indforstået med henvendelse</t>
   </si>
   <si>
     <t>253bbdc0-c4ca-4e77-9d3e-3a9e51281636</t>
   </si>
   <si>
-    <t>M�l/form�l</t>
+    <t>Mål/formål</t>
   </si>
   <si>
     <t>416fe27d-3ccf-4390-8742-8b52a9d8dc78</t>
   </si>
   <si>
-    <t>FFB borgers m�l og �nsker</t>
-  </si>
-  <si>
-    <t>Borgers m�l og �nsker som specificeret af FFB. Det er overordnet og er som udtrykt af borger</t>
+    <t>FFB borgers mål og ønsker</t>
+  </si>
+  <si>
+    <t>Borgers mål og ønsker som specificeret af FFB. Det er overordnet og er som udtrykt af borger</t>
   </si>
   <si>
     <t>6746d4af-145a-4bfd-a672-05c0cf11b53b</t>
   </si>
   <si>
-    <t>FFB delm�l</t>
-  </si>
-  <si>
-    <t>Delm�l i FFB, ligger under indsatsm�l, og er som udtrykt af udf�rer</t>
+    <t>FFB delmål</t>
+  </si>
+  <si>
+    <t>Delmål i FFB, ligger under indsatsmål, og er som udtrykt af udfører</t>
   </si>
   <si>
     <t>0bb3daef-538d-45dc-b444-abdbcb63f6bc</t>
   </si>
   <si>
-    <t>FFB indsatsm�l</t>
-  </si>
-  <si>
-    <t>Indsatsm�l i FFB - er de konkrete faglige m�l der arbejdes med, og som er knyttet til tilstande og opf�lgninger</t>
+    <t>FFB indsatsmål</t>
+  </si>
+  <si>
+    <t>Indsatsmål i FFB - er de konkrete faglige mål der arbejdes med, og som er knyttet til tilstande og opfølgninger</t>
+  </si>
+  <si>
+    <t>ffb9886b-d04e-46b1-9165-a400f91f822b</t>
+  </si>
+  <si>
+    <t>FSIII borgers ønsker og mål</t>
   </si>
   <si>
     <t>ca552020-6ed1-4cdc-b0d4-32697f1f27ad</t>
   </si>
   <si>
-    <t>FSIII tilstandsm�l</t>
-  </si>
-  <si>
-    <t>Tilstandsm�l som defineret af FSIII - ofte i form af en forventet tilstand</t>
+    <t>FSIII tilstandsmål</t>
+  </si>
+  <si>
+    <t>Tilstandsmål som defineret af FSIII - ofte i form af en forventet tilstand</t>
   </si>
   <si>
     <t>424827b1-23aa-4848-962b-56ee47def560</t>
   </si>
   <si>
-    <t>Indsatsform�l</t>
-  </si>
-  <si>
-    <t>Det overordnede form�l med hele indsatsen (Defineret af FFB men bruges ogs� for FSIII)</t>
-  </si>
-  <si>
-    <t>ffb9886b-d04e-46b1-9165-a400f91f822b</t>
-  </si>
-  <si>
-    <t>Borgers �nsker og m�l</t>
+    <t>Indsatsformål</t>
+  </si>
+  <si>
+    <t>Det overordnede formål med hele indsatsen (Defineret af FFB men bruges også for FSIII)</t>
+  </si>
+  <si>
+    <t>11266a8f-5795-42ab-88ec-4fe5c6c28e80</t>
+  </si>
+  <si>
+    <t>målfokus</t>
+  </si>
+  <si>
+    <t>66959f77-6e2a-4574-8423-3ff097f8b9fa</t>
+  </si>
+  <si>
+    <t>funktionsevneniveau</t>
+  </si>
+  <si>
+    <t>målet udtrykkes i form af et funktionsevneniveau, som kan være et FFB funktionsevneniveau eller FSIII tilstandsniveau</t>
+  </si>
+  <si>
+    <t>90c48f03-f194-4b2f-ad7d-6cba1069ae48</t>
+  </si>
+  <si>
+    <t>måltype</t>
+  </si>
+  <si>
+    <t>målet udtrykkes i form af en måltype, måltypen er den forventede ændring i tilstanden givet indsatsen</t>
   </si>
   <si>
     <t>940f37e6-8a3d-483b-adac-be8af3268a5b</t>
@@ -495,10 +465,10 @@
     <t>95e787e0-5490-437d-ae4c-f3736644242f</t>
   </si>
   <si>
-    <t>afklarende samtale �119, FSIII</t>
-  </si>
-  <si>
-    <t>udf�relse af afklarende samtale vedr. sundhedsfremme og forebyggelse j�vnf�r FSIII</t>
+    <t>afklarende samtale §119, FSIII</t>
+  </si>
+  <si>
+    <t>udførelse af afklarende samtale vedr. sundhedsfremme og forebyggelse jævnfør FSIII</t>
   </si>
   <si>
     <t>e5a73b0e-a5d2-430e-931f-6156306ab00f</t>
@@ -507,7 +477,16 @@
     <t>funktionsevnevurdering hjemmepleje, FSIII</t>
   </si>
   <si>
-    <t>udf�relse af funktionsevnevurdering i hjemmeplejen j�vnf�r FSIII</t>
+    <t>udførelse af funktionsevnevurdering i hjemmeplejen jævnfør FSIII</t>
+  </si>
+  <si>
+    <t>e70c66c0-a939-493b-8ea8-5b7e7b48ba1a</t>
+  </si>
+  <si>
+    <t>generelle oplysninger, FSIII</t>
+  </si>
+  <si>
+    <t>indhentning af generelle oplysninger jævnfør FSIII</t>
   </si>
   <si>
     <t>f8ebd11a-04f3-4aa0-9786-406e8896c84d</t>
@@ -516,7 +495,7 @@
     <t>socialfaglig udredning, VUM/FFB</t>
   </si>
   <si>
-    <t>udf�relse af socialfaglig udredning som specificeret af VUM og FFB</t>
+    <t>udførelse af socialfaglig udredning som specificeret af VUM og FFB</t>
   </si>
   <si>
     <t>47fd1468-89da-4803-9d7a-ecc039a30d92</t>
@@ -525,7 +504,7 @@
     <t>sygeplejefaglig udredning, FSIII</t>
   </si>
   <si>
-    <t>udf�relse af sygeplejefaglig udredning j�vnf�r FSIII</t>
+    <t>udførelse af sygeplejefaglig udredning jævnfør FSIII</t>
   </si>
   <si>
     <t>0f0f223c-abe3-4720-aab8-c257679a0a4e</t>
@@ -534,94 +513,91 @@
     <t>terapeutfaglig udredning, FSIII</t>
   </si>
   <si>
-    <t>udf�relse af terapeutfaglig udredning j�vnf�r FSIII</t>
-  </si>
-  <si>
-    <t>e70c66c0-a939-493b-8ea8-5b7e7b48ba1a</t>
-  </si>
-  <si>
-    <t>generelle oplysninger, FSIII</t>
-  </si>
-  <si>
-    <t>indhentning af generelle oplysninger j�vnf�r FSIII</t>
+    <t>udførelse af terapeutfaglig udredning jævnfør FSIII</t>
   </si>
   <si>
     <t>10deb210-e7e1-4d56-9531-b9ff2102126e</t>
   </si>
   <si>
-    <t>Planlagt indsatsforl�b</t>
+    <t>Planlagt indsatsforløb</t>
   </si>
   <si>
     <t>e459386d-1474-4c31-89c5-c8bc7a25e3d4</t>
   </si>
   <si>
-    <t>Det planlagte indsatsforl�b er en social indsats, som defineret af FFB, med tilh�rende ydelser, m�lgruppe og tilbud</t>
+    <t>Det planlagte indsatsforløb er en social indsats, som defineret af FFB, med tilhørende ydelser, målgruppe og tilbud</t>
   </si>
   <si>
     <t>4fd6c23a-6ff3-4251-ac37-3ca095027b5b</t>
   </si>
   <si>
-    <t>Det planlagte indsatsforl�b vedr�rer sundhedsfremme og forebyggelse efter �119.</t>
+    <t>Sundhedsfremme og forebyggelse §119</t>
+  </si>
+  <si>
+    <t>Det planlagte indsatsforløb vedrører sundhedsfremme og forebyggelse efter §119</t>
   </si>
   <si>
     <t>5c160c02-e858-4c1f-925a-71ed64844749</t>
   </si>
   <si>
-    <t>Interventionsforl�b efter �119</t>
-  </si>
-  <si>
-    <t>Et planlagt �119 indsatsforl�b, som udelukkende indeholder interventioner, og som leveres samlet. Med interventioner menes indsatser, der s�ger at forbedre borgers tilstand. For �119 kunne et interventionsforl�b fx v�re et KOL-tr�ningshold der indeholder indsatserne fysisk tr�ning og funktionstr�ning.</t>
+    <t>Interventionsforløb efter §119</t>
+  </si>
+  <si>
+    <t>Et planlagt §119 indsatsforløb, som udelukkende indeholder interventioner, og som leveres samlet. Med interventioner menes indsatser, der søger at forbedre borgers tilstand. For §119 kunne et interventionsforløb fx være et KOL-træningshold der indeholder indsatserne fysisk træning og funktionstræning.</t>
   </si>
   <si>
     <t>9791e55a-656f-47eb-8fd5-c4a06b0a4662</t>
   </si>
   <si>
-    <t>Opf�lgningsforl�b efter �119</t>
-  </si>
-  <si>
-    <t>Planlagt indsatsforl�b der best�r af opf�lgningsindsatser. Anvendes hvis der i forvejen planl�gges opf�lgning ved flere forskellige lejligheder fx efter 2,4 og 6 m�neder.</t>
+    <t>Opfølgningsforløb efter §119</t>
+  </si>
+  <si>
+    <t>Planlagt indsatsforløb der består af opfølgningsindsatser. Anvendes hvis der i forvejen planlægges opfølgning ved flere forskellige lejligheder fx efter 2,4 og 6 måneder.</t>
   </si>
   <si>
     <t>ddd2f670-5ec7-4f9c-9a2c-aee25cb133bf</t>
   </si>
   <si>
-    <t>Det planlagte indsatsforl�b er genoptr�ning efter sundhedslovens �140.</t>
+    <t>Genoptræning efter §140</t>
+  </si>
+  <si>
+    <t>Det planlagte indsatsforløb er genoptræning efter sundhedslovens §140</t>
   </si>
   <si>
     <t>f15b2663-94d9-4d0c-a5de-d8bd8e1e4ebb</t>
   </si>
   <si>
-    <t>Interventionsforl�b efter �140</t>
-  </si>
-  <si>
-    <t>Et planlagt �140 indsatsforl�b, som udelukkende indeholder interventioner, og som leveres samlet. Med interventioner menes indsatser, der s�ger at forbedre borgers tilstand. For �140 kunne et interventionsforl�b fx v�re et Kn�-genoptr�ningshold der indeholder indsatserne fysisk tr�ning, funktionstr�ning og vejledning og undervisning.</t>
+    <t>Interventionsforløb efter §140</t>
+  </si>
+  <si>
+    <t>Et planlagt §140 indsatsforløb, som udelukkende indeholder interventioner, og som leveres samlet. Med interventioner menes indsatser, der søger at forbedre borgers tilstand. For §140 kunne et interventionsforløb fx være et Knæ-genoptræningshold der indeholder indsatserne fysisk træning, funktionstræning og vejledning og undervisning.</t>
   </si>
   <si>
     <t>4863001e-14c7-4be8-a2da-e4f21a4b6ac4</t>
   </si>
   <si>
-    <t>Opf�lgningsforl�b efter �140</t>
-  </si>
-  <si>
-    <t>Planlagt indsatsforl�b efter �140 der best�r af opf�lgningsindsatser. Anvendes hvis der i forvejen planl�gges opf�lgning ved flere forskellige lejligheder fx efter 2,4 og 6 m�neder.</t>
+    <t>Opfølgningsforløb efter §140</t>
+  </si>
+  <si>
+    <t>Planlagt indsatsforløb efter §140 der består af opfølgningsindsatser. Anvendes hvis der i forvejen planlægges opfølgning ved flere forskellige lejligheder fx efter 2,4 og 6 måneder.</t>
   </si>
   <si>
     <t>2c059407-fed5-4852-92d8-6bb5ad63d7bb</t>
   </si>
   <si>
-    <t>Begrundelse for indsatsoph�r</t>
-  </si>
-  <si>
-    <t>Begrundelse for, at kommunale indsatser oph�rer</t>
+    <t>Begrundelse for indsatsophør</t>
+  </si>
+  <si>
+    <t>Begrundelse for, at kommunale indsatser ophører</t>
   </si>
   <si>
     <t>82e99421-31da-4915-96ed-168ccfa1d20c</t>
   </si>
   <si>
-    <t>H�ndelse medf�rer oph�r</t>
-  </si>
-  <si>
-    <t>H�ndelse, som ikke er et aktivt fravalg eller en behovsvurdering medf�rer oph�r. Det kan fx v�re en l�ngere hospitalsindl�ggelse, eller at borger flytter.</t>
+    <t>Hændelse medfører ophør</t>
+  </si>
+  <si>
+    <t>Hændelse, som ikke er et aktivt fravalg eller en behovsvurdering medfører ophør. Det kan fx være en længere hospitalsindlæggelse, eller at borger flytter.</t>
   </si>
   <si>
     <t>4bbf6d6a-a1c6-41c2-b8c1-7352b7378adf</t>
@@ -630,7 +606,7 @@
     <t>Ikke yderligere behov (borger-vurderet)</t>
   </si>
   <si>
-    <t>Borger vurderer, at han/hun ikke har yderligere behov og afslutter derfor f�r tid</t>
+    <t>Borger vurderer, at han/hun ikke har yderligere behov og afslutter derfor før tid</t>
   </si>
   <si>
     <t>a63b6aa6-7d56-4e67-a5b3-d73f6d262af5</t>
@@ -639,7 +615,7 @@
     <t>Ikke yderligere behov (fagperson-vurderet)</t>
   </si>
   <si>
-    <t>Fagperson vurderer, at borger ikke har yderligere behov og afslutter derfor f�r tid</t>
+    <t>Fagperson vurderer, at borger ikke har yderligere behov og afslutter derfor før tid</t>
   </si>
   <si>
     <t>3a5a72b7-addf-4857-b80c-04e4246e3072</t>
@@ -666,22 +642,22 @@
     <t>Aktivt fravalg pga. logistik ifm. transport</t>
   </si>
   <si>
-    <t>Borger har behov, men har foretaget et aktivt fravalg pga. den logistiske udfordring det er mht. transport, at n� frem til det sted indsatsen tilbydes</t>
+    <t>Borger har behov, men har foretaget et aktivt fravalg pga. den logistiske udfordring det er mht. transport, at nå frem til det sted indsatsen tilbydes</t>
   </si>
   <si>
     <t>a3f2bd01-078b-486e-81be-797d192ad7bd</t>
   </si>
   <si>
-    <t>Aktivt fravalg pga. anden tr�ning</t>
-  </si>
-  <si>
-    <t>Borger har behov, men har foretaget et aktivt fravalg fordi han/hun er p�begyndt tr�ning i andet regi fx fitnesscenter</t>
+    <t>Aktivt fravalg pga. anden træning</t>
+  </si>
+  <si>
+    <t>Borger har behov, men har foretaget et aktivt fravalg fordi han/hun er påbegyndt træning i andet regi fx fitnesscenter</t>
   </si>
   <si>
     <t>f8436c2e-af1c-44fe-939d-473b518dd01d</t>
   </si>
   <si>
-    <t>Aktivt fravalg pga. �konomi ifm. transport</t>
+    <t>Aktivt fravalg pga. økonomi ifm. transport</t>
   </si>
   <si>
     <t>Borger har behov, men har foretaget et aktivt fravalg pga. den omkostning der er forbundet med transport til det sted indsatsen tilbydes</t>
@@ -712,57 +688,6 @@
   </si>
   <si>
     <t>Indsats leveres individuelt</t>
-  </si>
-  <si>
-    <t>bf469e95-f9e3-45c7-bf15-ab7e8a85236f</t>
-  </si>
-  <si>
-    <t>Kontaktklasse</t>
-  </si>
-  <si>
-    <t>Type af kontakt. Beskriver leveringsmetode.</t>
-  </si>
-  <si>
-    <t>1b55a4b0-1156-4f58-b2df-b5c6014d9048</t>
-  </si>
-  <si>
-    <t>Telefonisk</t>
-  </si>
-  <si>
-    <t>Kontakten er foreg�et per telefon.</t>
-  </si>
-  <si>
-    <t>124be95d-6924-4609-9d2a-e7c73ae3ab3d</t>
-  </si>
-  <si>
-    <t>Sk�rmbes�g</t>
-  </si>
-  <si>
-    <t>Kontakten er foreg�et via sk�rm med mulighed for t�ndt kamera, s� parterne har haft mulighed for at interagere ansigt til ansigt, og fremvise ting.</t>
-  </si>
-  <si>
-    <t>11266a8f-5795-42ab-88ec-4fe5c6c28e80</t>
-  </si>
-  <si>
-    <t>M�lfokus</t>
-  </si>
-  <si>
-    <t>66959f77-6e2a-4574-8423-3ff097f8b9fa</t>
-  </si>
-  <si>
-    <t>funktionsevneniveau</t>
-  </si>
-  <si>
-    <t>m�let udtrykkes i form af et funktionsevneniveau, som kan v�re et FFB funktionsevneniveau eller FSIII tilstandsniveau</t>
-  </si>
-  <si>
-    <t>90c48f03-f194-4b2f-ad7d-6cba1069ae48</t>
-  </si>
-  <si>
-    <t>m�ltype</t>
-  </si>
-  <si>
-    <t>m�let udtrykkes i form af en m�ltype, m�ltypen er den forventede �ndring i tilstanden givet indsatsen</t>
   </si>
 </sst>
 </file>
@@ -1067,7 +992,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D75"/>
+  <dimension ref="A1:D66"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1140,7 +1065,7 @@
         <v>49</v>
       </c>
       <c r="D5" t="s" s="2">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6">
@@ -1148,13 +1073,13 @@
         <v>41</v>
       </c>
       <c r="B6" t="s" s="2">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C6" t="s" s="2">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D6" t="s" s="2">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7">
@@ -1162,10 +1087,10 @@
         <v>41</v>
       </c>
       <c r="B7" t="s" s="2">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C7" t="s" s="2">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D7" t="s" s="2">
         <v>54</v>
@@ -1257,7 +1182,7 @@
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B14" t="s" s="2">
         <v>72</v>
@@ -1271,7 +1196,7 @@
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B15" t="s" s="2">
         <v>75</v>
@@ -1313,30 +1238,30 @@
     </row>
     <row r="18">
       <c r="A18" t="s" s="2">
-        <v>41</v>
+        <v>84</v>
       </c>
       <c r="B18" t="s" s="2">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C18" t="s" s="2">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D18" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="2">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B19" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C19" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D19" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20">
@@ -1344,13 +1269,13 @@
         <v>41</v>
       </c>
       <c r="B20" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C20" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D20" t="s" s="2">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="21">
@@ -1358,13 +1283,13 @@
         <v>41</v>
       </c>
       <c r="B21" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C21" t="s" s="2">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D21" t="s" s="2">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="22">
@@ -1372,13 +1297,13 @@
         <v>41</v>
       </c>
       <c r="B22" t="s" s="2">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C22" t="s" s="2">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D22" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="23">
@@ -1386,18 +1311,18 @@
         <v>41</v>
       </c>
       <c r="B23" t="s" s="2">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C23" t="s" s="2">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D23" t="s" s="2">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="2">
-        <v>102</v>
+        <v>41</v>
       </c>
       <c r="B24" t="s" s="2">
         <v>103</v>
@@ -1411,7 +1336,7 @@
     </row>
     <row r="25">
       <c r="A25" t="s" s="2">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B25" t="s" s="2">
         <v>106</v>
@@ -1439,7 +1364,7 @@
     </row>
     <row r="27">
       <c r="A27" t="s" s="2">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B27" t="s" s="2">
         <v>112</v>
@@ -1448,7 +1373,7 @@
         <v>113</v>
       </c>
       <c r="D27" t="s" s="2">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="28">
@@ -1456,13 +1381,13 @@
         <v>41</v>
       </c>
       <c r="B28" t="s" s="2">
+        <v>114</v>
+      </c>
+      <c r="C28" t="s" s="2">
         <v>115</v>
       </c>
-      <c r="C28" t="s" s="2">
+      <c r="D28" t="s" s="2">
         <v>116</v>
-      </c>
-      <c r="D28" t="s" s="2">
-        <v>117</v>
       </c>
     </row>
     <row r="29">
@@ -1470,27 +1395,27 @@
         <v>41</v>
       </c>
       <c r="B29" t="s" s="2">
+        <v>117</v>
+      </c>
+      <c r="C29" t="s" s="2">
         <v>118</v>
       </c>
-      <c r="C29" t="s" s="2">
+      <c r="D29" t="s" s="2">
         <v>119</v>
-      </c>
-      <c r="D29" t="s" s="2">
-        <v>120</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="2">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B30" t="s" s="2">
+        <v>120</v>
+      </c>
+      <c r="C30" t="s" s="2">
         <v>121</v>
       </c>
-      <c r="C30" t="s" s="2">
-        <v>122</v>
-      </c>
       <c r="D30" t="s" s="2">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="31">
@@ -1498,13 +1423,13 @@
         <v>41</v>
       </c>
       <c r="B31" t="s" s="2">
+        <v>122</v>
+      </c>
+      <c r="C31" t="s" s="2">
+        <v>123</v>
+      </c>
+      <c r="D31" t="s" s="2">
         <v>124</v>
-      </c>
-      <c r="C31" t="s" s="2">
-        <v>125</v>
-      </c>
-      <c r="D31" t="s" s="2">
-        <v>126</v>
       </c>
     </row>
     <row r="32">
@@ -1512,27 +1437,27 @@
         <v>41</v>
       </c>
       <c r="B32" t="s" s="2">
+        <v>125</v>
+      </c>
+      <c r="C32" t="s" s="2">
+        <v>126</v>
+      </c>
+      <c r="D32" t="s" s="2">
         <v>127</v>
-      </c>
-      <c r="C32" t="s" s="2">
-        <v>128</v>
-      </c>
-      <c r="D32" t="s" s="2">
-        <v>129</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="2">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B33" t="s" s="2">
+        <v>128</v>
+      </c>
+      <c r="C33" t="s" s="2">
+        <v>129</v>
+      </c>
+      <c r="D33" t="s" s="2">
         <v>130</v>
-      </c>
-      <c r="C33" t="s" s="2">
-        <v>131</v>
-      </c>
-      <c r="D33" t="s" s="2">
-        <v>131</v>
       </c>
     </row>
     <row r="34">
@@ -1540,13 +1465,13 @@
         <v>41</v>
       </c>
       <c r="B34" t="s" s="2">
+        <v>131</v>
+      </c>
+      <c r="C34" t="s" s="2">
         <v>132</v>
       </c>
-      <c r="C34" t="s" s="2">
-        <v>133</v>
-      </c>
       <c r="D34" t="s" s="2">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="35">
@@ -1554,41 +1479,41 @@
         <v>41</v>
       </c>
       <c r="B35" t="s" s="2">
+        <v>133</v>
+      </c>
+      <c r="C35" t="s" s="2">
+        <v>134</v>
+      </c>
+      <c r="D35" t="s" s="2">
         <v>135</v>
-      </c>
-      <c r="C35" t="s" s="2">
-        <v>136</v>
-      </c>
-      <c r="D35" t="s" s="2">
-        <v>137</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="2">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B36" t="s" s="2">
+        <v>136</v>
+      </c>
+      <c r="C36" t="s" s="2">
+        <v>137</v>
+      </c>
+      <c r="D36" t="s" s="2">
         <v>138</v>
-      </c>
-      <c r="C36" t="s" s="2">
-        <v>139</v>
-      </c>
-      <c r="D36" t="s" s="2">
-        <v>139</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="2">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B37" t="s" s="2">
+        <v>139</v>
+      </c>
+      <c r="C37" t="s" s="2">
         <v>140</v>
       </c>
-      <c r="C37" t="s" s="2">
-        <v>141</v>
-      </c>
       <c r="D37" t="s" s="2">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="38">
@@ -1596,13 +1521,13 @@
         <v>41</v>
       </c>
       <c r="B38" t="s" s="2">
+        <v>141</v>
+      </c>
+      <c r="C38" t="s" s="2">
+        <v>142</v>
+      </c>
+      <c r="D38" t="s" s="2">
         <v>143</v>
-      </c>
-      <c r="C38" t="s" s="2">
-        <v>144</v>
-      </c>
-      <c r="D38" t="s" s="2">
-        <v>145</v>
       </c>
     </row>
     <row r="39">
@@ -1610,27 +1535,27 @@
         <v>41</v>
       </c>
       <c r="B39" t="s" s="2">
+        <v>144</v>
+      </c>
+      <c r="C39" t="s" s="2">
+        <v>145</v>
+      </c>
+      <c r="D39" t="s" s="2">
         <v>146</v>
-      </c>
-      <c r="C39" t="s" s="2">
-        <v>147</v>
-      </c>
-      <c r="D39" t="s" s="2">
-        <v>148</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="2">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B40" t="s" s="2">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C40" t="s" s="2">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D40" t="s" s="2">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="41">
@@ -1638,13 +1563,13 @@
         <v>41</v>
       </c>
       <c r="B41" t="s" s="2">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C41" t="s" s="2">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D41" t="s" s="2">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="42">
@@ -1652,27 +1577,27 @@
         <v>41</v>
       </c>
       <c r="B42" t="s" s="2">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C42" t="s" s="2">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D42" t="s" s="2">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="2">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B43" t="s" s="2">
+        <v>155</v>
+      </c>
+      <c r="C43" t="s" s="2">
+        <v>156</v>
+      </c>
+      <c r="D43" t="s" s="2">
         <v>157</v>
-      </c>
-      <c r="C43" t="s" s="2">
-        <v>158</v>
-      </c>
-      <c r="D43" t="s" s="2">
-        <v>158</v>
       </c>
     </row>
     <row r="44">
@@ -1680,13 +1605,13 @@
         <v>41</v>
       </c>
       <c r="B44" t="s" s="2">
+        <v>158</v>
+      </c>
+      <c r="C44" t="s" s="2">
         <v>159</v>
       </c>
-      <c r="C44" t="s" s="2">
+      <c r="D44" t="s" s="2">
         <v>160</v>
-      </c>
-      <c r="D44" t="s" s="2">
-        <v>161</v>
       </c>
     </row>
     <row r="45">
@@ -1694,13 +1619,13 @@
         <v>41</v>
       </c>
       <c r="B45" t="s" s="2">
+        <v>161</v>
+      </c>
+      <c r="C45" t="s" s="2">
         <v>162</v>
       </c>
-      <c r="C45" t="s" s="2">
+      <c r="D45" t="s" s="2">
         <v>163</v>
-      </c>
-      <c r="D45" t="s" s="2">
-        <v>164</v>
       </c>
     </row>
     <row r="46">
@@ -1708,27 +1633,27 @@
         <v>41</v>
       </c>
       <c r="B46" t="s" s="2">
+        <v>164</v>
+      </c>
+      <c r="C46" t="s" s="2">
         <v>165</v>
       </c>
-      <c r="C46" t="s" s="2">
+      <c r="D46" t="s" s="2">
         <v>166</v>
-      </c>
-      <c r="D46" t="s" s="2">
-        <v>167</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s" s="2">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B47" t="s" s="2">
+        <v>167</v>
+      </c>
+      <c r="C47" t="s" s="2">
         <v>168</v>
       </c>
-      <c r="C47" t="s" s="2">
-        <v>169</v>
-      </c>
       <c r="D47" t="s" s="2">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="48">
@@ -1736,13 +1661,13 @@
         <v>41</v>
       </c>
       <c r="B48" t="s" s="2">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C48" t="s" s="2">
-        <v>172</v>
+        <v>64</v>
       </c>
       <c r="D48" t="s" s="2">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="49">
@@ -1750,41 +1675,41 @@
         <v>41</v>
       </c>
       <c r="B49" t="s" s="2">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C49" t="s" s="2">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D49" t="s" s="2">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s" s="2">
-        <v>38</v>
+        <v>84</v>
       </c>
       <c r="B50" t="s" s="2">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C50" t="s" s="2">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D50" t="s" s="2">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s" s="2">
-        <v>41</v>
+        <v>84</v>
       </c>
       <c r="B51" t="s" s="2">
+        <v>177</v>
+      </c>
+      <c r="C51" t="s" s="2">
+        <v>178</v>
+      </c>
+      <c r="D51" t="s" s="2">
         <v>179</v>
-      </c>
-      <c r="C51" t="s" s="2">
-        <v>58</v>
-      </c>
-      <c r="D51" t="s" s="2">
-        <v>180</v>
       </c>
     </row>
     <row r="52">
@@ -1792,10 +1717,10 @@
         <v>41</v>
       </c>
       <c r="B52" t="s" s="2">
+        <v>180</v>
+      </c>
+      <c r="C52" t="s" s="2">
         <v>181</v>
-      </c>
-      <c r="C52" t="s" s="2">
-        <v>67</v>
       </c>
       <c r="D52" t="s" s="2">
         <v>182</v>
@@ -1803,7 +1728,7 @@
     </row>
     <row r="53">
       <c r="A53" t="s" s="2">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="B53" t="s" s="2">
         <v>183</v>
@@ -1817,7 +1742,7 @@
     </row>
     <row r="54">
       <c r="A54" t="s" s="2">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="B54" t="s" s="2">
         <v>186</v>
@@ -1831,58 +1756,58 @@
     </row>
     <row r="55">
       <c r="A55" t="s" s="2">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B55" t="s" s="2">
         <v>189</v>
       </c>
       <c r="C55" t="s" s="2">
-        <v>70</v>
+        <v>190</v>
       </c>
       <c r="D55" t="s" s="2">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s" s="2">
-        <v>102</v>
+        <v>41</v>
       </c>
       <c r="B56" t="s" s="2">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C56" t="s" s="2">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D56" t="s" s="2">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s" s="2">
-        <v>102</v>
+        <v>41</v>
       </c>
       <c r="B57" t="s" s="2">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C57" t="s" s="2">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D57" t="s" s="2">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s" s="2">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B58" t="s" s="2">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C58" t="s" s="2">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D58" t="s" s="2">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="59">
@@ -1890,237 +1815,111 @@
         <v>41</v>
       </c>
       <c r="B59" t="s" s="2">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C59" t="s" s="2">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D59" t="s" s="2">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s" s="2">
-        <v>41</v>
+        <v>84</v>
       </c>
       <c r="B60" t="s" s="2">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C60" t="s" s="2">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D60" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s" s="2">
-        <v>41</v>
+        <v>84</v>
       </c>
       <c r="B61" t="s" s="2">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C61" t="s" s="2">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D61" t="s" s="2">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s" s="2">
-        <v>41</v>
+        <v>84</v>
       </c>
       <c r="B62" t="s" s="2">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C62" t="s" s="2">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D62" t="s" s="2">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s" s="2">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="B63" t="s" s="2">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C63" t="s" s="2">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D63" t="s" s="2">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s" s="2">
-        <v>102</v>
+        <v>38</v>
       </c>
       <c r="B64" t="s" s="2">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C64" t="s" s="2">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D64" t="s" s="2">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s" s="2">
-        <v>102</v>
+        <v>41</v>
       </c>
       <c r="B65" t="s" s="2">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C65" t="s" s="2">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D65" t="s" s="2">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s" s="2">
-        <v>102</v>
+        <v>41</v>
       </c>
       <c r="B66" t="s" s="2">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C66" t="s" s="2">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="D66" t="s" s="2">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="B67" t="s" s="2">
         <v>224</v>
-      </c>
-      <c r="C67" t="s" s="2">
-        <v>225</v>
-      </c>
-      <c r="D67" t="s" s="2">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="B68" t="s" s="2">
-        <v>227</v>
-      </c>
-      <c r="C68" t="s" s="2">
-        <v>228</v>
-      </c>
-      <c r="D68" t="s" s="2">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="B69" t="s" s="2">
-        <v>230</v>
-      </c>
-      <c r="C69" t="s" s="2">
-        <v>231</v>
-      </c>
-      <c r="D69" t="s" s="2">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="B70" t="s" s="2">
-        <v>233</v>
-      </c>
-      <c r="C70" t="s" s="2">
-        <v>234</v>
-      </c>
-      <c r="D70" t="s" s="2">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="B71" t="s" s="2">
-        <v>236</v>
-      </c>
-      <c r="C71" t="s" s="2">
-        <v>237</v>
-      </c>
-      <c r="D71" t="s" s="2">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="B72" t="s" s="2">
-        <v>239</v>
-      </c>
-      <c r="C72" t="s" s="2">
-        <v>240</v>
-      </c>
-      <c r="D72" t="s" s="2">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="B73" t="s" s="2">
-        <v>242</v>
-      </c>
-      <c r="C73" t="s" s="2">
-        <v>243</v>
-      </c>
-      <c r="D73" t="s" s="2">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="B74" t="s" s="2">
-        <v>244</v>
-      </c>
-      <c r="C74" t="s" s="2">
-        <v>245</v>
-      </c>
-      <c r="D74" t="s" s="2">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="B75" t="s" s="2">
-        <v>247</v>
-      </c>
-      <c r="C75" t="s" s="2">
-        <v>248</v>
-      </c>
-      <c r="D75" t="s" s="2">
-        <v>249</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding term 2.0 now utf-8
</commit_message>
<xml_diff>
--- a/term/CodeSystem-CareSocialCodes.xlsx
+++ b/term/CodeSystem-CareSocialCodes.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="250">
   <si>
     <t>Property</t>
   </si>
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>1.1.0</t>
+    <t>2.0.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-07-10T23:08:03+02:00</t>
+    <t>2024-06-03T10:45:43+02:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -69,13 +69,13 @@
     <t>Contact</t>
   </si>
   <si>
-    <t>No display for ContactDetail</t>
+    <t>Kommunernes Landsforening (http://kl.dk)</t>
   </si>
   <si>
     <t>Description</t>
   </si>
   <si>
-    <t>Administrative/technical codes in Local Govenment Denmark (KL), associated with KLCommonCareSocial</t>
+    <t>Administrative/technical codes in Local Govenment Denmark (KL), associated with common use cases across areas or kl-core</t>
   </si>
   <si>
     <t>Purpose</t>
@@ -159,6 +159,18 @@
     <t>Vurdering der sammenholder oplysninger fra udredning mhp en samlet faglig analyse og konklusion.</t>
   </si>
   <si>
+    <t>3f7a8ca0-afca-4b0d-8773-a99b5f2f8aaf</t>
+  </si>
+  <si>
+    <t>VUM Borgerens perspektiv på indsatsen</t>
+  </si>
+  <si>
+    <t>f52887de-023f-4193-b6b0-4b0a37b1cffc</t>
+  </si>
+  <si>
+    <t>VUM Borgerens ressourcer i forhold til indsatsen</t>
+  </si>
+  <si>
     <t>54c4ffea-7caf-4edc-8aa9-ef6e0be26c4c</t>
   </si>
   <si>
@@ -168,67 +180,64 @@
     <t>Sagsvurdering, der sammenholder resultaterne af en myndighedsudredning og den øvrige sagsoplysning med henblik på at træffe en afgørelse</t>
   </si>
   <si>
-    <t>3f7a8ca0-afca-4b0d-8773-a99b5f2f8aaf</t>
-  </si>
-  <si>
-    <t>VUM Borgerens perspektiv på indsatsen</t>
-  </si>
-  <si>
-    <t>f52887de-023f-4193-b6b0-4b0a37b1cffc</t>
-  </si>
-  <si>
-    <t>VUM Borgerens ressourcer i forhold til indsatsen</t>
-  </si>
-  <si>
     <t>7b41185e-eeb4-437d-8120-5d51bbd27a79</t>
   </si>
   <si>
     <t>Indsats/ydelses-anmodning</t>
   </si>
   <si>
+    <t>4a297733-4d66-4726-a933-590d55cf91e0</t>
+  </si>
+  <si>
+    <t>Social indsats</t>
+  </si>
+  <si>
+    <t>Der anmodes om en social indsats</t>
+  </si>
+  <si>
     <t>ad865929-7363-4b2d-a271-01993181fbaf</t>
   </si>
   <si>
-    <t>Hjemmepleje</t>
-  </si>
-  <si>
-    <t>Der anmodes om hjemmepleje</t>
+    <t>Kommunal pleje og omsorg</t>
+  </si>
+  <si>
+    <t>Der anmodes om kommunal pleje og omsorg fx hjemmepleje til ældre borger.</t>
   </si>
   <si>
     <t>490ab7be-ddb1-4a54-baf1-009fe6e8a83b</t>
   </si>
   <si>
-    <t>Hjemmesygepleje</t>
-  </si>
-  <si>
-    <t>Der anmodes om sygepleje</t>
-  </si>
-  <si>
-    <t>4a297733-4d66-4726-a933-590d55cf91e0</t>
-  </si>
-  <si>
-    <t>Social indsats</t>
-  </si>
-  <si>
-    <t>Der anmodes om en social indsats</t>
+    <t>Kommunal sygepleje</t>
+  </si>
+  <si>
+    <t>Der anmodes om kommunal sygepleje.</t>
   </si>
   <si>
     <t>a71921ea-fe83-441d-933b-cc21d0b3c8c3</t>
   </si>
   <si>
-    <t>Sundhedsfremme og forebyggelse</t>
-  </si>
-  <si>
-    <t>Der anmodes om sundhedsfremme og forebyggelse</t>
+    <t>Kommunal Sundhedsfremme og forebyggelse</t>
+  </si>
+  <si>
+    <t>Der anmodes om kommunal sundhedsfremme og forebyggelse efter SUL §119.</t>
   </si>
   <si>
     <t>7fc66c15-0cb3-4c89-9e18-f3a01e6a6592</t>
   </si>
   <si>
-    <t>Træning</t>
-  </si>
-  <si>
-    <t>Der anmodes om træning</t>
+    <t>Kommunal genoptræning efter sygehusophold</t>
+  </si>
+  <si>
+    <t>Der anmodes om kommunal genoptræning efter sygehusophold efter SUL §140.</t>
+  </si>
+  <si>
+    <t>d267ac44-8d7f-43e9-8535-ab3da350649f</t>
+  </si>
+  <si>
+    <t>Kommunalt hjælpemiddelområde</t>
+  </si>
+  <si>
+    <t>Der anmodes om hjælpemidler og lignende, der ligger indenfor det kommunale hjælpemiddelområde dvs § 112, § 113, § 114, § 116 i Serviceloven.</t>
   </si>
   <si>
     <t>b5731132-f6b9-4a47-995d-681d2b755d4f</t>
@@ -258,13 +267,58 @@
     <t>Sagsbehandler er kilde til oplysning eller vurdering</t>
   </si>
   <si>
+    <t>329774f9-7700-47cf-9c00-63765d9e8078</t>
+  </si>
+  <si>
+    <t>Medarbejder og pårørende alene</t>
+  </si>
+  <si>
+    <t>En medarbejder og pårørende er sammen, men uden input fra borger, kilde til oplysning eller vurdering. Fx PUF spørgeskema i sundhedsplejen.</t>
+  </si>
+  <si>
+    <t>8fe80acb-2c2a-4f10-b2b8-ddb77d2f69dc</t>
+  </si>
+  <si>
+    <t>Medarbejder alene</t>
+  </si>
+  <si>
+    <t>Medarbejderen er alene kilde til oplysning eller vurdering. Fx AIMS skema i sundhedsplejen.</t>
+  </si>
+  <si>
+    <t>12428e48-7df8-441f-9a89-d92bb7874066</t>
+  </si>
+  <si>
+    <t>Borger støttet af medarbejder</t>
+  </si>
+  <si>
+    <t>Borger fik hjælp af en medarbejder til at komme med oplysninger eller vurderinger. Fx ældre borger der får hjælp til at udfylde WHO5 spørgeskema.</t>
+  </si>
+  <si>
+    <t>b66dc78a-a673-43fc-8ac0-1e859ba626e0</t>
+  </si>
+  <si>
+    <t>Borger støttet af pårørende</t>
+  </si>
+  <si>
+    <t>Borger fik hjælp af en pårørende til at komme med oplysninger eller vurderinger. Fx ældre borger der får hjælp til at udfylde WHO5 spørgeskema.</t>
+  </si>
+  <si>
+    <t>166d2437-4e47-4a52-bd94-cdbe91086ca6</t>
+  </si>
+  <si>
+    <t>Pårørende alene</t>
+  </si>
+  <si>
+    <t>Pårørende er alene, uden input fra borger, kilde til oplysninger eller vuderderinger. Fx WHO 5 spørgeskema for svækket ældre borger udfyldt af datter.</t>
+  </si>
+  <si>
     <t>63338442-7b2e-405b-acc0-142361ef19f1</t>
   </si>
   <si>
     <t>Andre</t>
   </si>
   <si>
-    <t>Andre end borger og sagsbehandler er kilde til oplysning eller vurdering. Fx læge, pårørende og udfører</t>
+    <t>Andre end borger og sagsbehandler er kilde til oplysning eller vurdering. Fx læge, pårørende og udfører. Denne definition af andre, bruges kun på voksensocialområdet.</t>
   </si>
   <si>
     <t>3</t>
@@ -408,34 +462,289 @@
     <t>Indsatsmål i FFB - er de konkrete faglige mål der arbejdes med, og som er knyttet til tilstande og opfølgninger</t>
   </si>
   <si>
+    <t>ca552020-6ed1-4cdc-b0d4-32697f1f27ad</t>
+  </si>
+  <si>
+    <t>FSIII tilstandsmål</t>
+  </si>
+  <si>
+    <t>Tilstandsmål som defineret af FSIII - ofte i form af en forventet tilstand</t>
+  </si>
+  <si>
+    <t>424827b1-23aa-4848-962b-56ee47def560</t>
+  </si>
+  <si>
+    <t>Indsatsformål</t>
+  </si>
+  <si>
+    <t>Det overordnede formål med hele indsatsen (Defineret af FFB men bruges også for FSIII)</t>
+  </si>
+  <si>
     <t>ffb9886b-d04e-46b1-9165-a400f91f822b</t>
   </si>
   <si>
-    <t>FSIII borgers ønsker og mål</t>
-  </si>
-  <si>
-    <t>ca552020-6ed1-4cdc-b0d4-32697f1f27ad</t>
-  </si>
-  <si>
-    <t>FSIII tilstandsmål</t>
-  </si>
-  <si>
-    <t>Tilstandsmål som defineret af FSIII - ofte i form af en forventet tilstand</t>
-  </si>
-  <si>
-    <t>424827b1-23aa-4848-962b-56ee47def560</t>
-  </si>
-  <si>
-    <t>Indsatsformål</t>
-  </si>
-  <si>
-    <t>Det overordnede formål med hele indsatsen (Defineret af FFB men bruges også for FSIII)</t>
+    <t>Borgers ønsker og mål</t>
+  </si>
+  <si>
+    <t>940f37e6-8a3d-483b-adac-be8af3268a5b</t>
+  </si>
+  <si>
+    <t>oplysningsaktivitet</t>
+  </si>
+  <si>
+    <t>95e787e0-5490-437d-ae4c-f3736644242f</t>
+  </si>
+  <si>
+    <t>afklarende samtale §119, FSIII</t>
+  </si>
+  <si>
+    <t>udførelse af afklarende samtale vedr. sundhedsfremme og forebyggelse jævnfør FSIII</t>
+  </si>
+  <si>
+    <t>e5a73b0e-a5d2-430e-931f-6156306ab00f</t>
+  </si>
+  <si>
+    <t>funktionsevnevurdering hjemmepleje, FSIII</t>
+  </si>
+  <si>
+    <t>udførelse af funktionsevnevurdering i hjemmeplejen jævnfør FSIII</t>
+  </si>
+  <si>
+    <t>f8ebd11a-04f3-4aa0-9786-406e8896c84d</t>
+  </si>
+  <si>
+    <t>socialfaglig udredning, VUM/FFB</t>
+  </si>
+  <si>
+    <t>udførelse af socialfaglig udredning som specificeret af VUM og FFB</t>
+  </si>
+  <si>
+    <t>47fd1468-89da-4803-9d7a-ecc039a30d92</t>
+  </si>
+  <si>
+    <t>sygeplejefaglig udredning, FSIII</t>
+  </si>
+  <si>
+    <t>udførelse af sygeplejefaglig udredning jævnfør FSIII</t>
+  </si>
+  <si>
+    <t>0f0f223c-abe3-4720-aab8-c257679a0a4e</t>
+  </si>
+  <si>
+    <t>terapeutfaglig udredning, FSIII</t>
+  </si>
+  <si>
+    <t>udførelse af terapeutfaglig udredning jævnfør FSIII</t>
+  </si>
+  <si>
+    <t>e70c66c0-a939-493b-8ea8-5b7e7b48ba1a</t>
+  </si>
+  <si>
+    <t>generelle oplysninger, FSIII</t>
+  </si>
+  <si>
+    <t>indhentning af generelle oplysninger jævnfør FSIII</t>
+  </si>
+  <si>
+    <t>10deb210-e7e1-4d56-9531-b9ff2102126e</t>
+  </si>
+  <si>
+    <t>Planlagt indsatsforløb</t>
+  </si>
+  <si>
+    <t>e459386d-1474-4c31-89c5-c8bc7a25e3d4</t>
+  </si>
+  <si>
+    <t>Det planlagte indsatsforløb er en social indsats, som defineret af FFB, med tilhørende ydelser, målgruppe og tilbud</t>
+  </si>
+  <si>
+    <t>4fd6c23a-6ff3-4251-ac37-3ca095027b5b</t>
+  </si>
+  <si>
+    <t>Det planlagte indsatsforløb vedrører sundhedsfremme og forebyggelse efter §119.</t>
+  </si>
+  <si>
+    <t>5c160c02-e858-4c1f-925a-71ed64844749</t>
+  </si>
+  <si>
+    <t>Interventionsforløb efter §119</t>
+  </si>
+  <si>
+    <t>Et planlagt §119 indsatsforløb, som udelukkende indeholder interventioner, og som leveres samlet. Med interventioner menes indsatser, der søger at forbedre borgers tilstand. For §119 kunne et interventionsforløb fx være et KOL-træningshold der indeholder indsatserne fysisk træning og funktionstræning.</t>
+  </si>
+  <si>
+    <t>9791e55a-656f-47eb-8fd5-c4a06b0a4662</t>
+  </si>
+  <si>
+    <t>Opfølgningsforløb efter §119</t>
+  </si>
+  <si>
+    <t>Planlagt indsatsforløb der består af opfølgningsindsatser. Anvendes hvis der i forvejen planlægges opfølgning ved flere forskellige lejligheder fx efter 2,4 og 6 måneder.</t>
+  </si>
+  <si>
+    <t>ddd2f670-5ec7-4f9c-9a2c-aee25cb133bf</t>
+  </si>
+  <si>
+    <t>Det planlagte indsatsforløb er genoptræning efter sundhedslovens §140.</t>
+  </si>
+  <si>
+    <t>f15b2663-94d9-4d0c-a5de-d8bd8e1e4ebb</t>
+  </si>
+  <si>
+    <t>Interventionsforløb efter §140</t>
+  </si>
+  <si>
+    <t>Et planlagt §140 indsatsforløb, som udelukkende indeholder interventioner, og som leveres samlet. Med interventioner menes indsatser, der søger at forbedre borgers tilstand. For §140 kunne et interventionsforløb fx være et Knæ-genoptræningshold der indeholder indsatserne fysisk træning, funktionstræning og vejledning og undervisning.</t>
+  </si>
+  <si>
+    <t>4863001e-14c7-4be8-a2da-e4f21a4b6ac4</t>
+  </si>
+  <si>
+    <t>Opfølgningsforløb efter §140</t>
+  </si>
+  <si>
+    <t>Planlagt indsatsforløb efter §140 der består af opfølgningsindsatser. Anvendes hvis der i forvejen planlægges opfølgning ved flere forskellige lejligheder fx efter 2,4 og 6 måneder.</t>
+  </si>
+  <si>
+    <t>2c059407-fed5-4852-92d8-6bb5ad63d7bb</t>
+  </si>
+  <si>
+    <t>Begrundelse for indsatsophør</t>
+  </si>
+  <si>
+    <t>Begrundelse for, at kommunale indsatser ophører</t>
+  </si>
+  <si>
+    <t>82e99421-31da-4915-96ed-168ccfa1d20c</t>
+  </si>
+  <si>
+    <t>Hændelse medfører ophør</t>
+  </si>
+  <si>
+    <t>Hændelse, som ikke er et aktivt fravalg eller en behovsvurdering medfører ophør. Det kan fx være en længere hospitalsindlæggelse, eller at borger flytter.</t>
+  </si>
+  <si>
+    <t>4bbf6d6a-a1c6-41c2-b8c1-7352b7378adf</t>
+  </si>
+  <si>
+    <t>Ikke yderligere behov (borger-vurderet)</t>
+  </si>
+  <si>
+    <t>Borger vurderer, at han/hun ikke har yderligere behov og afslutter derfor før tid</t>
+  </si>
+  <si>
+    <t>a63b6aa6-7d56-4e67-a5b3-d73f6d262af5</t>
+  </si>
+  <si>
+    <t>Ikke yderligere behov (fagperson-vurderet)</t>
+  </si>
+  <si>
+    <t>Fagperson vurderer, at borger ikke har yderligere behov og afslutter derfor før tid</t>
+  </si>
+  <si>
+    <t>3a5a72b7-addf-4857-b80c-04e4246e3072</t>
+  </si>
+  <si>
+    <t>Aktivt fravalg</t>
+  </si>
+  <si>
+    <t>Borger har behov, men har foretaget et aktivt fravalg</t>
+  </si>
+  <si>
+    <t>0cd5734d-b663-47c6-a3da-6b14a937d144</t>
+  </si>
+  <si>
+    <t>Aktivt fravalg pga. anden sygdom</t>
+  </si>
+  <si>
+    <t>Borger har behov, men har foretaget et aktivt fravalg pga. anden sygdom</t>
+  </si>
+  <si>
+    <t>8371b769-4bfb-4ac8-b130-d91c54784a56</t>
+  </si>
+  <si>
+    <t>Aktivt fravalg pga. logistik ifm. transport</t>
+  </si>
+  <si>
+    <t>Borger har behov, men har foretaget et aktivt fravalg pga. den logistiske udfordring det er mht. transport, at nå frem til det sted indsatsen tilbydes</t>
+  </si>
+  <si>
+    <t>a3f2bd01-078b-486e-81be-797d192ad7bd</t>
+  </si>
+  <si>
+    <t>Aktivt fravalg pga. anden træning</t>
+  </si>
+  <si>
+    <t>Borger har behov, men har foretaget et aktivt fravalg fordi han/hun er påbegyndt træning i andet regi fx fitnesscenter</t>
+  </si>
+  <si>
+    <t>f8436c2e-af1c-44fe-939d-473b518dd01d</t>
+  </si>
+  <si>
+    <t>Aktivt fravalg pga. økonomi ifm. transport</t>
+  </si>
+  <si>
+    <t>Borger har behov, men har foretaget et aktivt fravalg pga. den omkostning der er forbundet med transport til det sted indsatsen tilbydes</t>
+  </si>
+  <si>
+    <t>3f79cee2-b148-4f2c-9cbd-387820e74685</t>
+  </si>
+  <si>
+    <t>Leveringstype</t>
+  </si>
+  <si>
+    <t>Om der leveres individuelt eller gruppebaseret</t>
+  </si>
+  <si>
+    <t>2865f123-15a7-4a36-a514-32ea37c400ca</t>
+  </si>
+  <si>
+    <t>Gruppebaseret indsats</t>
+  </si>
+  <si>
+    <t>Indsats leveres i gruppe</t>
+  </si>
+  <si>
+    <t>8d12d74c-17da-47a7-a4fe-e69dbaec0a8c</t>
+  </si>
+  <si>
+    <t>Individuel indsats</t>
+  </si>
+  <si>
+    <t>Indsats leveres individuelt</t>
+  </si>
+  <si>
+    <t>bf469e95-f9e3-45c7-bf15-ab7e8a85236f</t>
+  </si>
+  <si>
+    <t>Kontaktklasse</t>
+  </si>
+  <si>
+    <t>Type af kontakt. Beskriver leveringsmetode.</t>
+  </si>
+  <si>
+    <t>1b55a4b0-1156-4f58-b2df-b5c6014d9048</t>
+  </si>
+  <si>
+    <t>Telefonisk</t>
+  </si>
+  <si>
+    <t>Kontakten er foregået per telefon.</t>
+  </si>
+  <si>
+    <t>124be95d-6924-4609-9d2a-e7c73ae3ab3d</t>
+  </si>
+  <si>
+    <t>Skærmbesøg</t>
+  </si>
+  <si>
+    <t>Kontakten er foregået via skærm med mulighed for tændt kamera, så parterne har haft mulighed for at interagere ansigt til ansigt, og fremvise ting.</t>
   </si>
   <si>
     <t>11266a8f-5795-42ab-88ec-4fe5c6c28e80</t>
   </si>
   <si>
-    <t>målfokus</t>
+    <t>Målfokus</t>
   </si>
   <si>
     <t>66959f77-6e2a-4574-8423-3ff097f8b9fa</t>
@@ -454,240 +763,6 @@
   </si>
   <si>
     <t>målet udtrykkes i form af en måltype, måltypen er den forventede ændring i tilstanden givet indsatsen</t>
-  </si>
-  <si>
-    <t>940f37e6-8a3d-483b-adac-be8af3268a5b</t>
-  </si>
-  <si>
-    <t>oplysningsaktivitet</t>
-  </si>
-  <si>
-    <t>95e787e0-5490-437d-ae4c-f3736644242f</t>
-  </si>
-  <si>
-    <t>afklarende samtale §119, FSIII</t>
-  </si>
-  <si>
-    <t>udførelse af afklarende samtale vedr. sundhedsfremme og forebyggelse jævnfør FSIII</t>
-  </si>
-  <si>
-    <t>e5a73b0e-a5d2-430e-931f-6156306ab00f</t>
-  </si>
-  <si>
-    <t>funktionsevnevurdering hjemmepleje, FSIII</t>
-  </si>
-  <si>
-    <t>udførelse af funktionsevnevurdering i hjemmeplejen jævnfør FSIII</t>
-  </si>
-  <si>
-    <t>e70c66c0-a939-493b-8ea8-5b7e7b48ba1a</t>
-  </si>
-  <si>
-    <t>generelle oplysninger, FSIII</t>
-  </si>
-  <si>
-    <t>indhentning af generelle oplysninger jævnfør FSIII</t>
-  </si>
-  <si>
-    <t>f8ebd11a-04f3-4aa0-9786-406e8896c84d</t>
-  </si>
-  <si>
-    <t>socialfaglig udredning, VUM/FFB</t>
-  </si>
-  <si>
-    <t>udførelse af socialfaglig udredning som specificeret af VUM og FFB</t>
-  </si>
-  <si>
-    <t>47fd1468-89da-4803-9d7a-ecc039a30d92</t>
-  </si>
-  <si>
-    <t>sygeplejefaglig udredning, FSIII</t>
-  </si>
-  <si>
-    <t>udførelse af sygeplejefaglig udredning jævnfør FSIII</t>
-  </si>
-  <si>
-    <t>0f0f223c-abe3-4720-aab8-c257679a0a4e</t>
-  </si>
-  <si>
-    <t>terapeutfaglig udredning, FSIII</t>
-  </si>
-  <si>
-    <t>udførelse af terapeutfaglig udredning jævnfør FSIII</t>
-  </si>
-  <si>
-    <t>10deb210-e7e1-4d56-9531-b9ff2102126e</t>
-  </si>
-  <si>
-    <t>Planlagt indsatsforløb</t>
-  </si>
-  <si>
-    <t>e459386d-1474-4c31-89c5-c8bc7a25e3d4</t>
-  </si>
-  <si>
-    <t>Det planlagte indsatsforløb er en social indsats, som defineret af FFB, med tilhørende ydelser, målgruppe og tilbud</t>
-  </si>
-  <si>
-    <t>4fd6c23a-6ff3-4251-ac37-3ca095027b5b</t>
-  </si>
-  <si>
-    <t>Sundhedsfremme og forebyggelse §119</t>
-  </si>
-  <si>
-    <t>Det planlagte indsatsforløb vedrører sundhedsfremme og forebyggelse efter §119</t>
-  </si>
-  <si>
-    <t>5c160c02-e858-4c1f-925a-71ed64844749</t>
-  </si>
-  <si>
-    <t>Interventionsforløb efter §119</t>
-  </si>
-  <si>
-    <t>Et planlagt §119 indsatsforløb, som udelukkende indeholder interventioner, og som leveres samlet. Med interventioner menes indsatser, der søger at forbedre borgers tilstand. For §119 kunne et interventionsforløb fx være et KOL-træningshold der indeholder indsatserne fysisk træning og funktionstræning.</t>
-  </si>
-  <si>
-    <t>9791e55a-656f-47eb-8fd5-c4a06b0a4662</t>
-  </si>
-  <si>
-    <t>Opfølgningsforløb efter §119</t>
-  </si>
-  <si>
-    <t>Planlagt indsatsforløb der består af opfølgningsindsatser. Anvendes hvis der i forvejen planlægges opfølgning ved flere forskellige lejligheder fx efter 2,4 og 6 måneder.</t>
-  </si>
-  <si>
-    <t>ddd2f670-5ec7-4f9c-9a2c-aee25cb133bf</t>
-  </si>
-  <si>
-    <t>Genoptræning efter §140</t>
-  </si>
-  <si>
-    <t>Det planlagte indsatsforløb er genoptræning efter sundhedslovens §140</t>
-  </si>
-  <si>
-    <t>f15b2663-94d9-4d0c-a5de-d8bd8e1e4ebb</t>
-  </si>
-  <si>
-    <t>Interventionsforløb efter §140</t>
-  </si>
-  <si>
-    <t>Et planlagt §140 indsatsforløb, som udelukkende indeholder interventioner, og som leveres samlet. Med interventioner menes indsatser, der søger at forbedre borgers tilstand. For §140 kunne et interventionsforløb fx være et Knæ-genoptræningshold der indeholder indsatserne fysisk træning, funktionstræning og vejledning og undervisning.</t>
-  </si>
-  <si>
-    <t>4863001e-14c7-4be8-a2da-e4f21a4b6ac4</t>
-  </si>
-  <si>
-    <t>Opfølgningsforløb efter §140</t>
-  </si>
-  <si>
-    <t>Planlagt indsatsforløb efter §140 der består af opfølgningsindsatser. Anvendes hvis der i forvejen planlægges opfølgning ved flere forskellige lejligheder fx efter 2,4 og 6 måneder.</t>
-  </si>
-  <si>
-    <t>2c059407-fed5-4852-92d8-6bb5ad63d7bb</t>
-  </si>
-  <si>
-    <t>Begrundelse for indsatsophør</t>
-  </si>
-  <si>
-    <t>Begrundelse for, at kommunale indsatser ophører</t>
-  </si>
-  <si>
-    <t>82e99421-31da-4915-96ed-168ccfa1d20c</t>
-  </si>
-  <si>
-    <t>Hændelse medfører ophør</t>
-  </si>
-  <si>
-    <t>Hændelse, som ikke er et aktivt fravalg eller en behovsvurdering medfører ophør. Det kan fx være en længere hospitalsindlæggelse, eller at borger flytter.</t>
-  </si>
-  <si>
-    <t>4bbf6d6a-a1c6-41c2-b8c1-7352b7378adf</t>
-  </si>
-  <si>
-    <t>Ikke yderligere behov (borger-vurderet)</t>
-  </si>
-  <si>
-    <t>Borger vurderer, at han/hun ikke har yderligere behov og afslutter derfor før tid</t>
-  </si>
-  <si>
-    <t>a63b6aa6-7d56-4e67-a5b3-d73f6d262af5</t>
-  </si>
-  <si>
-    <t>Ikke yderligere behov (fagperson-vurderet)</t>
-  </si>
-  <si>
-    <t>Fagperson vurderer, at borger ikke har yderligere behov og afslutter derfor før tid</t>
-  </si>
-  <si>
-    <t>3a5a72b7-addf-4857-b80c-04e4246e3072</t>
-  </si>
-  <si>
-    <t>Aktivt fravalg</t>
-  </si>
-  <si>
-    <t>Borger har behov, men har foretaget et aktivt fravalg</t>
-  </si>
-  <si>
-    <t>0cd5734d-b663-47c6-a3da-6b14a937d144</t>
-  </si>
-  <si>
-    <t>Aktivt fravalg pga. anden sygdom</t>
-  </si>
-  <si>
-    <t>Borger har behov, men har foretaget et aktivt fravalg pga. anden sygdom</t>
-  </si>
-  <si>
-    <t>8371b769-4bfb-4ac8-b130-d91c54784a56</t>
-  </si>
-  <si>
-    <t>Aktivt fravalg pga. logistik ifm. transport</t>
-  </si>
-  <si>
-    <t>Borger har behov, men har foretaget et aktivt fravalg pga. den logistiske udfordring det er mht. transport, at nå frem til det sted indsatsen tilbydes</t>
-  </si>
-  <si>
-    <t>a3f2bd01-078b-486e-81be-797d192ad7bd</t>
-  </si>
-  <si>
-    <t>Aktivt fravalg pga. anden træning</t>
-  </si>
-  <si>
-    <t>Borger har behov, men har foretaget et aktivt fravalg fordi han/hun er påbegyndt træning i andet regi fx fitnesscenter</t>
-  </si>
-  <si>
-    <t>f8436c2e-af1c-44fe-939d-473b518dd01d</t>
-  </si>
-  <si>
-    <t>Aktivt fravalg pga. økonomi ifm. transport</t>
-  </si>
-  <si>
-    <t>Borger har behov, men har foretaget et aktivt fravalg pga. den omkostning der er forbundet med transport til det sted indsatsen tilbydes</t>
-  </si>
-  <si>
-    <t>3f79cee2-b148-4f2c-9cbd-387820e74685</t>
-  </si>
-  <si>
-    <t>Leveringstype</t>
-  </si>
-  <si>
-    <t>Om der leveres individuelt eller gruppebaseret</t>
-  </si>
-  <si>
-    <t>2865f123-15a7-4a36-a514-32ea37c400ca</t>
-  </si>
-  <si>
-    <t>Gruppebaseret indsats</t>
-  </si>
-  <si>
-    <t>Indsats leveres i gruppe</t>
-  </si>
-  <si>
-    <t>8d12d74c-17da-47a7-a4fe-e69dbaec0a8c</t>
-  </si>
-  <si>
-    <t>Individuel indsats</t>
-  </si>
-  <si>
-    <t>Indsats leveres individuelt</t>
   </si>
 </sst>
 </file>
@@ -992,7 +1067,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D66"/>
+  <dimension ref="A1:D75"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1065,7 +1140,7 @@
         <v>49</v>
       </c>
       <c r="D5" t="s" s="2">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6">
@@ -1073,13 +1148,13 @@
         <v>41</v>
       </c>
       <c r="B6" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="C6" t="s" s="2">
         <v>51</v>
       </c>
-      <c r="C6" t="s" s="2">
-        <v>52</v>
-      </c>
       <c r="D6" t="s" s="2">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7">
@@ -1087,10 +1162,10 @@
         <v>41</v>
       </c>
       <c r="B7" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="C7" t="s" s="2">
         <v>53</v>
-      </c>
-      <c r="C7" t="s" s="2">
-        <v>54</v>
       </c>
       <c r="D7" t="s" s="2">
         <v>54</v>
@@ -1182,7 +1257,7 @@
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B14" t="s" s="2">
         <v>72</v>
@@ -1196,7 +1271,7 @@
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B15" t="s" s="2">
         <v>75</v>
@@ -1238,30 +1313,30 @@
     </row>
     <row r="18">
       <c r="A18" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="B18" t="s" s="2">
         <v>84</v>
       </c>
-      <c r="B18" t="s" s="2">
+      <c r="C18" t="s" s="2">
         <v>85</v>
       </c>
-      <c r="C18" t="s" s="2">
+      <c r="D18" t="s" s="2">
         <v>86</v>
-      </c>
-      <c r="D18" t="s" s="2">
-        <v>87</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="2">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B19" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="C19" t="s" s="2">
         <v>88</v>
       </c>
-      <c r="C19" t="s" s="2">
+      <c r="D19" t="s" s="2">
         <v>89</v>
-      </c>
-      <c r="D19" t="s" s="2">
-        <v>90</v>
       </c>
     </row>
     <row r="20">
@@ -1269,13 +1344,13 @@
         <v>41</v>
       </c>
       <c r="B20" t="s" s="2">
+        <v>90</v>
+      </c>
+      <c r="C20" t="s" s="2">
         <v>91</v>
       </c>
-      <c r="C20" t="s" s="2">
+      <c r="D20" t="s" s="2">
         <v>92</v>
-      </c>
-      <c r="D20" t="s" s="2">
-        <v>93</v>
       </c>
     </row>
     <row r="21">
@@ -1283,13 +1358,13 @@
         <v>41</v>
       </c>
       <c r="B21" t="s" s="2">
+        <v>93</v>
+      </c>
+      <c r="C21" t="s" s="2">
         <v>94</v>
       </c>
-      <c r="C21" t="s" s="2">
+      <c r="D21" t="s" s="2">
         <v>95</v>
-      </c>
-      <c r="D21" t="s" s="2">
-        <v>96</v>
       </c>
     </row>
     <row r="22">
@@ -1297,13 +1372,13 @@
         <v>41</v>
       </c>
       <c r="B22" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="C22" t="s" s="2">
         <v>97</v>
       </c>
-      <c r="C22" t="s" s="2">
+      <c r="D22" t="s" s="2">
         <v>98</v>
-      </c>
-      <c r="D22" t="s" s="2">
-        <v>99</v>
       </c>
     </row>
     <row r="23">
@@ -1311,18 +1386,18 @@
         <v>41</v>
       </c>
       <c r="B23" t="s" s="2">
+        <v>99</v>
+      </c>
+      <c r="C23" t="s" s="2">
         <v>100</v>
       </c>
-      <c r="C23" t="s" s="2">
+      <c r="D23" t="s" s="2">
         <v>101</v>
-      </c>
-      <c r="D23" t="s" s="2">
-        <v>102</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="2">
-        <v>41</v>
+        <v>102</v>
       </c>
       <c r="B24" t="s" s="2">
         <v>103</v>
@@ -1336,7 +1411,7 @@
     </row>
     <row r="25">
       <c r="A25" t="s" s="2">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B25" t="s" s="2">
         <v>106</v>
@@ -1364,7 +1439,7 @@
     </row>
     <row r="27">
       <c r="A27" t="s" s="2">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B27" t="s" s="2">
         <v>112</v>
@@ -1373,7 +1448,7 @@
         <v>113</v>
       </c>
       <c r="D27" t="s" s="2">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="28">
@@ -1381,13 +1456,13 @@
         <v>41</v>
       </c>
       <c r="B28" t="s" s="2">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C28" t="s" s="2">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D28" t="s" s="2">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="29">
@@ -1395,27 +1470,27 @@
         <v>41</v>
       </c>
       <c r="B29" t="s" s="2">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C29" t="s" s="2">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D29" t="s" s="2">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="2">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B30" t="s" s="2">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C30" t="s" s="2">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D30" t="s" s="2">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="31">
@@ -1423,13 +1498,13 @@
         <v>41</v>
       </c>
       <c r="B31" t="s" s="2">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C31" t="s" s="2">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D31" t="s" s="2">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="32">
@@ -1437,27 +1512,27 @@
         <v>41</v>
       </c>
       <c r="B32" t="s" s="2">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C32" t="s" s="2">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D32" t="s" s="2">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="2">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B33" t="s" s="2">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C33" t="s" s="2">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="D33" t="s" s="2">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="34">
@@ -1465,13 +1540,13 @@
         <v>41</v>
       </c>
       <c r="B34" t="s" s="2">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C34" t="s" s="2">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D34" t="s" s="2">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="35">
@@ -1479,41 +1554,41 @@
         <v>41</v>
       </c>
       <c r="B35" t="s" s="2">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C35" t="s" s="2">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="D35" t="s" s="2">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="2">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B36" t="s" s="2">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C36" t="s" s="2">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D36" t="s" s="2">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="2">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B37" t="s" s="2">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C37" t="s" s="2">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D37" t="s" s="2">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="38">
@@ -1521,13 +1596,13 @@
         <v>41</v>
       </c>
       <c r="B38" t="s" s="2">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C38" t="s" s="2">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D38" t="s" s="2">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="39">
@@ -1535,27 +1610,27 @@
         <v>41</v>
       </c>
       <c r="B39" t="s" s="2">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C39" t="s" s="2">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D39" t="s" s="2">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="2">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B40" t="s" s="2">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="C40" t="s" s="2">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D40" t="s" s="2">
-        <v>148</v>
+        <v>151</v>
       </c>
     </row>
     <row r="41">
@@ -1563,13 +1638,13 @@
         <v>41</v>
       </c>
       <c r="B41" t="s" s="2">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="C41" t="s" s="2">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="D41" t="s" s="2">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
     <row r="42">
@@ -1577,27 +1652,27 @@
         <v>41</v>
       </c>
       <c r="B42" t="s" s="2">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="C42" t="s" s="2">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="D42" t="s" s="2">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="2">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B43" t="s" s="2">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C43" t="s" s="2">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D43" t="s" s="2">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="44">
@@ -1605,13 +1680,13 @@
         <v>41</v>
       </c>
       <c r="B44" t="s" s="2">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C44" t="s" s="2">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D44" t="s" s="2">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="45">
@@ -1619,13 +1694,13 @@
         <v>41</v>
       </c>
       <c r="B45" t="s" s="2">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C45" t="s" s="2">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D45" t="s" s="2">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="46">
@@ -1633,27 +1708,27 @@
         <v>41</v>
       </c>
       <c r="B46" t="s" s="2">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C46" t="s" s="2">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D46" t="s" s="2">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s" s="2">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B47" t="s" s="2">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C47" t="s" s="2">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D47" t="s" s="2">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="48">
@@ -1661,13 +1736,13 @@
         <v>41</v>
       </c>
       <c r="B48" t="s" s="2">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="C48" t="s" s="2">
-        <v>64</v>
+        <v>172</v>
       </c>
       <c r="D48" t="s" s="2">
-        <v>170</v>
+        <v>173</v>
       </c>
     </row>
     <row r="49">
@@ -1675,41 +1750,41 @@
         <v>41</v>
       </c>
       <c r="B49" t="s" s="2">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="C49" t="s" s="2">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="D49" t="s" s="2">
-        <v>173</v>
+        <v>176</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s" s="2">
-        <v>84</v>
+        <v>38</v>
       </c>
       <c r="B50" t="s" s="2">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="C50" t="s" s="2">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="D50" t="s" s="2">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s" s="2">
-        <v>84</v>
+        <v>41</v>
       </c>
       <c r="B51" t="s" s="2">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C51" t="s" s="2">
-        <v>178</v>
+        <v>58</v>
       </c>
       <c r="D51" t="s" s="2">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="52">
@@ -1717,10 +1792,10 @@
         <v>41</v>
       </c>
       <c r="B52" t="s" s="2">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C52" t="s" s="2">
-        <v>181</v>
+        <v>67</v>
       </c>
       <c r="D52" t="s" s="2">
         <v>182</v>
@@ -1728,7 +1803,7 @@
     </row>
     <row r="53">
       <c r="A53" t="s" s="2">
-        <v>84</v>
+        <v>102</v>
       </c>
       <c r="B53" t="s" s="2">
         <v>183</v>
@@ -1742,7 +1817,7 @@
     </row>
     <row r="54">
       <c r="A54" t="s" s="2">
-        <v>84</v>
+        <v>102</v>
       </c>
       <c r="B54" t="s" s="2">
         <v>186</v>
@@ -1756,58 +1831,58 @@
     </row>
     <row r="55">
       <c r="A55" t="s" s="2">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B55" t="s" s="2">
         <v>189</v>
       </c>
       <c r="C55" t="s" s="2">
+        <v>70</v>
+      </c>
+      <c r="D55" t="s" s="2">
         <v>190</v>
-      </c>
-      <c r="D55" t="s" s="2">
-        <v>191</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s" s="2">
-        <v>41</v>
+        <v>102</v>
       </c>
       <c r="B56" t="s" s="2">
+        <v>191</v>
+      </c>
+      <c r="C56" t="s" s="2">
         <v>192</v>
       </c>
-      <c r="C56" t="s" s="2">
+      <c r="D56" t="s" s="2">
         <v>193</v>
-      </c>
-      <c r="D56" t="s" s="2">
-        <v>194</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s" s="2">
-        <v>41</v>
+        <v>102</v>
       </c>
       <c r="B57" t="s" s="2">
+        <v>194</v>
+      </c>
+      <c r="C57" t="s" s="2">
         <v>195</v>
       </c>
-      <c r="C57" t="s" s="2">
+      <c r="D57" t="s" s="2">
         <v>196</v>
-      </c>
-      <c r="D57" t="s" s="2">
-        <v>197</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s" s="2">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B58" t="s" s="2">
+        <v>197</v>
+      </c>
+      <c r="C58" t="s" s="2">
         <v>198</v>
       </c>
-      <c r="C58" t="s" s="2">
+      <c r="D58" t="s" s="2">
         <v>199</v>
-      </c>
-      <c r="D58" t="s" s="2">
-        <v>200</v>
       </c>
     </row>
     <row r="59">
@@ -1815,111 +1890,237 @@
         <v>41</v>
       </c>
       <c r="B59" t="s" s="2">
+        <v>200</v>
+      </c>
+      <c r="C59" t="s" s="2">
         <v>201</v>
       </c>
-      <c r="C59" t="s" s="2">
+      <c r="D59" t="s" s="2">
         <v>202</v>
-      </c>
-      <c r="D59" t="s" s="2">
-        <v>203</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s" s="2">
-        <v>84</v>
+        <v>41</v>
       </c>
       <c r="B60" t="s" s="2">
+        <v>203</v>
+      </c>
+      <c r="C60" t="s" s="2">
         <v>204</v>
       </c>
-      <c r="C60" t="s" s="2">
+      <c r="D60" t="s" s="2">
         <v>205</v>
-      </c>
-      <c r="D60" t="s" s="2">
-        <v>206</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s" s="2">
-        <v>84</v>
+        <v>41</v>
       </c>
       <c r="B61" t="s" s="2">
+        <v>206</v>
+      </c>
+      <c r="C61" t="s" s="2">
         <v>207</v>
       </c>
-      <c r="C61" t="s" s="2">
+      <c r="D61" t="s" s="2">
         <v>208</v>
-      </c>
-      <c r="D61" t="s" s="2">
-        <v>209</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s" s="2">
-        <v>84</v>
+        <v>41</v>
       </c>
       <c r="B62" t="s" s="2">
+        <v>209</v>
+      </c>
+      <c r="C62" t="s" s="2">
         <v>210</v>
       </c>
-      <c r="C62" t="s" s="2">
+      <c r="D62" t="s" s="2">
         <v>211</v>
-      </c>
-      <c r="D62" t="s" s="2">
-        <v>212</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s" s="2">
-        <v>84</v>
+        <v>102</v>
       </c>
       <c r="B63" t="s" s="2">
+        <v>212</v>
+      </c>
+      <c r="C63" t="s" s="2">
         <v>213</v>
       </c>
-      <c r="C63" t="s" s="2">
+      <c r="D63" t="s" s="2">
         <v>214</v>
-      </c>
-      <c r="D63" t="s" s="2">
-        <v>215</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s" s="2">
-        <v>38</v>
+        <v>102</v>
       </c>
       <c r="B64" t="s" s="2">
+        <v>215</v>
+      </c>
+      <c r="C64" t="s" s="2">
         <v>216</v>
       </c>
-      <c r="C64" t="s" s="2">
+      <c r="D64" t="s" s="2">
         <v>217</v>
-      </c>
-      <c r="D64" t="s" s="2">
-        <v>218</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s" s="2">
-        <v>41</v>
+        <v>102</v>
       </c>
       <c r="B65" t="s" s="2">
+        <v>218</v>
+      </c>
+      <c r="C65" t="s" s="2">
         <v>219</v>
       </c>
-      <c r="C65" t="s" s="2">
+      <c r="D65" t="s" s="2">
         <v>220</v>
-      </c>
-      <c r="D65" t="s" s="2">
-        <v>221</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s" s="2">
-        <v>41</v>
+        <v>102</v>
       </c>
       <c r="B66" t="s" s="2">
+        <v>221</v>
+      </c>
+      <c r="C66" t="s" s="2">
         <v>222</v>
       </c>
-      <c r="C66" t="s" s="2">
+      <c r="D66" t="s" s="2">
         <v>223</v>
       </c>
-      <c r="D66" t="s" s="2">
+    </row>
+    <row r="67">
+      <c r="A67" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="B67" t="s" s="2">
         <v>224</v>
+      </c>
+      <c r="C67" t="s" s="2">
+        <v>225</v>
+      </c>
+      <c r="D67" t="s" s="2">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="B68" t="s" s="2">
+        <v>227</v>
+      </c>
+      <c r="C68" t="s" s="2">
+        <v>228</v>
+      </c>
+      <c r="D68" t="s" s="2">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="B69" t="s" s="2">
+        <v>230</v>
+      </c>
+      <c r="C69" t="s" s="2">
+        <v>231</v>
+      </c>
+      <c r="D69" t="s" s="2">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="B70" t="s" s="2">
+        <v>233</v>
+      </c>
+      <c r="C70" t="s" s="2">
+        <v>234</v>
+      </c>
+      <c r="D70" t="s" s="2">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="B71" t="s" s="2">
+        <v>236</v>
+      </c>
+      <c r="C71" t="s" s="2">
+        <v>237</v>
+      </c>
+      <c r="D71" t="s" s="2">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="B72" t="s" s="2">
+        <v>239</v>
+      </c>
+      <c r="C72" t="s" s="2">
+        <v>240</v>
+      </c>
+      <c r="D72" t="s" s="2">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="B73" t="s" s="2">
+        <v>242</v>
+      </c>
+      <c r="C73" t="s" s="2">
+        <v>243</v>
+      </c>
+      <c r="D73" t="s" s="2">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="B74" t="s" s="2">
+        <v>244</v>
+      </c>
+      <c r="C74" t="s" s="2">
+        <v>245</v>
+      </c>
+      <c r="D74" t="s" s="2">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="B75" t="s" s="2">
+        <v>247</v>
+      </c>
+      <c r="C75" t="s" s="2">
+        <v>248</v>
+      </c>
+      <c r="D75" t="s" s="2">
+        <v>249</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "adding term 2.0 now utf-8"
This reverts commit 78ae09ef7158944b5ce8ba326bcf0fbc536c742d.
</commit_message>
<xml_diff>
--- a/term/CodeSystem-CareSocialCodes.xlsx
+++ b/term/CodeSystem-CareSocialCodes.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="225">
   <si>
     <t>Property</t>
   </si>
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>2.0.0</t>
+    <t>1.1.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-06-03T10:45:43+02:00</t>
+    <t>2023-07-10T23:08:03+02:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -69,13 +69,13 @@
     <t>Contact</t>
   </si>
   <si>
-    <t>Kommunernes Landsforening (http://kl.dk)</t>
+    <t>No display for ContactDetail</t>
   </si>
   <si>
     <t>Description</t>
   </si>
   <si>
-    <t>Administrative/technical codes in Local Govenment Denmark (KL), associated with common use cases across areas or kl-core</t>
+    <t>Administrative/technical codes in Local Govenment Denmark (KL), associated with KLCommonCareSocial</t>
   </si>
   <si>
     <t>Purpose</t>
@@ -159,6 +159,15 @@
     <t>Vurdering der sammenholder oplysninger fra udredning mhp en samlet faglig analyse og konklusion.</t>
   </si>
   <si>
+    <t>54c4ffea-7caf-4edc-8aa9-ef6e0be26c4c</t>
+  </si>
+  <si>
+    <t>FSIII helhedsvurdering</t>
+  </si>
+  <si>
+    <t>Sagsvurdering, der sammenholder resultaterne af en myndighedsudredning og den øvrige sagsoplysning med henblik på at træffe en afgørelse</t>
+  </si>
+  <si>
     <t>3f7a8ca0-afca-4b0d-8773-a99b5f2f8aaf</t>
   </si>
   <si>
@@ -171,21 +180,30 @@
     <t>VUM Borgerens ressourcer i forhold til indsatsen</t>
   </si>
   <si>
-    <t>54c4ffea-7caf-4edc-8aa9-ef6e0be26c4c</t>
-  </si>
-  <si>
-    <t>FSIII helhedsvurdering</t>
-  </si>
-  <si>
-    <t>Sagsvurdering, der sammenholder resultaterne af en myndighedsudredning og den øvrige sagsoplysning med henblik på at træffe en afgørelse</t>
-  </si>
-  <si>
     <t>7b41185e-eeb4-437d-8120-5d51bbd27a79</t>
   </si>
   <si>
     <t>Indsats/ydelses-anmodning</t>
   </si>
   <si>
+    <t>ad865929-7363-4b2d-a271-01993181fbaf</t>
+  </si>
+  <si>
+    <t>Hjemmepleje</t>
+  </si>
+  <si>
+    <t>Der anmodes om hjemmepleje</t>
+  </si>
+  <si>
+    <t>490ab7be-ddb1-4a54-baf1-009fe6e8a83b</t>
+  </si>
+  <si>
+    <t>Hjemmesygepleje</t>
+  </si>
+  <si>
+    <t>Der anmodes om sygepleje</t>
+  </si>
+  <si>
     <t>4a297733-4d66-4726-a933-590d55cf91e0</t>
   </si>
   <si>
@@ -195,49 +213,22 @@
     <t>Der anmodes om en social indsats</t>
   </si>
   <si>
-    <t>ad865929-7363-4b2d-a271-01993181fbaf</t>
-  </si>
-  <si>
-    <t>Kommunal pleje og omsorg</t>
-  </si>
-  <si>
-    <t>Der anmodes om kommunal pleje og omsorg fx hjemmepleje til ældre borger.</t>
-  </si>
-  <si>
-    <t>490ab7be-ddb1-4a54-baf1-009fe6e8a83b</t>
-  </si>
-  <si>
-    <t>Kommunal sygepleje</t>
-  </si>
-  <si>
-    <t>Der anmodes om kommunal sygepleje.</t>
-  </si>
-  <si>
     <t>a71921ea-fe83-441d-933b-cc21d0b3c8c3</t>
   </si>
   <si>
-    <t>Kommunal Sundhedsfremme og forebyggelse</t>
-  </si>
-  <si>
-    <t>Der anmodes om kommunal sundhedsfremme og forebyggelse efter SUL §119.</t>
+    <t>Sundhedsfremme og forebyggelse</t>
+  </si>
+  <si>
+    <t>Der anmodes om sundhedsfremme og forebyggelse</t>
   </si>
   <si>
     <t>7fc66c15-0cb3-4c89-9e18-f3a01e6a6592</t>
   </si>
   <si>
-    <t>Kommunal genoptræning efter sygehusophold</t>
-  </si>
-  <si>
-    <t>Der anmodes om kommunal genoptræning efter sygehusophold efter SUL §140.</t>
-  </si>
-  <si>
-    <t>d267ac44-8d7f-43e9-8535-ab3da350649f</t>
-  </si>
-  <si>
-    <t>Kommunalt hjælpemiddelområde</t>
-  </si>
-  <si>
-    <t>Der anmodes om hjælpemidler og lignende, der ligger indenfor det kommunale hjælpemiddelområde dvs § 112, § 113, § 114, § 116 i Serviceloven.</t>
+    <t>Træning</t>
+  </si>
+  <si>
+    <t>Der anmodes om træning</t>
   </si>
   <si>
     <t>b5731132-f6b9-4a47-995d-681d2b755d4f</t>
@@ -267,58 +258,13 @@
     <t>Sagsbehandler er kilde til oplysning eller vurdering</t>
   </si>
   <si>
-    <t>329774f9-7700-47cf-9c00-63765d9e8078</t>
-  </si>
-  <si>
-    <t>Medarbejder og pårørende alene</t>
-  </si>
-  <si>
-    <t>En medarbejder og pårørende er sammen, men uden input fra borger, kilde til oplysning eller vurdering. Fx PUF spørgeskema i sundhedsplejen.</t>
-  </si>
-  <si>
-    <t>8fe80acb-2c2a-4f10-b2b8-ddb77d2f69dc</t>
-  </si>
-  <si>
-    <t>Medarbejder alene</t>
-  </si>
-  <si>
-    <t>Medarbejderen er alene kilde til oplysning eller vurdering. Fx AIMS skema i sundhedsplejen.</t>
-  </si>
-  <si>
-    <t>12428e48-7df8-441f-9a89-d92bb7874066</t>
-  </si>
-  <si>
-    <t>Borger støttet af medarbejder</t>
-  </si>
-  <si>
-    <t>Borger fik hjælp af en medarbejder til at komme med oplysninger eller vurderinger. Fx ældre borger der får hjælp til at udfylde WHO5 spørgeskema.</t>
-  </si>
-  <si>
-    <t>b66dc78a-a673-43fc-8ac0-1e859ba626e0</t>
-  </si>
-  <si>
-    <t>Borger støttet af pårørende</t>
-  </si>
-  <si>
-    <t>Borger fik hjælp af en pårørende til at komme med oplysninger eller vurderinger. Fx ældre borger der får hjælp til at udfylde WHO5 spørgeskema.</t>
-  </si>
-  <si>
-    <t>166d2437-4e47-4a52-bd94-cdbe91086ca6</t>
-  </si>
-  <si>
-    <t>Pårørende alene</t>
-  </si>
-  <si>
-    <t>Pårørende er alene, uden input fra borger, kilde til oplysninger eller vuderderinger. Fx WHO 5 spørgeskema for svækket ældre borger udfyldt af datter.</t>
-  </si>
-  <si>
     <t>63338442-7b2e-405b-acc0-142361ef19f1</t>
   </si>
   <si>
     <t>Andre</t>
   </si>
   <si>
-    <t>Andre end borger og sagsbehandler er kilde til oplysning eller vurdering. Fx læge, pårørende og udfører. Denne definition af andre, bruges kun på voksensocialområdet.</t>
+    <t>Andre end borger og sagsbehandler er kilde til oplysning eller vurdering. Fx læge, pårørende og udfører</t>
   </si>
   <si>
     <t>3</t>
@@ -462,6 +408,12 @@
     <t>Indsatsmål i FFB - er de konkrete faglige mål der arbejdes med, og som er knyttet til tilstande og opfølgninger</t>
   </si>
   <si>
+    <t>ffb9886b-d04e-46b1-9165-a400f91f822b</t>
+  </si>
+  <si>
+    <t>FSIII borgers ønsker og mål</t>
+  </si>
+  <si>
     <t>ca552020-6ed1-4cdc-b0d4-32697f1f27ad</t>
   </si>
   <si>
@@ -480,10 +432,28 @@
     <t>Det overordnede formål med hele indsatsen (Defineret af FFB men bruges også for FSIII)</t>
   </si>
   <si>
-    <t>ffb9886b-d04e-46b1-9165-a400f91f822b</t>
-  </si>
-  <si>
-    <t>Borgers ønsker og mål</t>
+    <t>11266a8f-5795-42ab-88ec-4fe5c6c28e80</t>
+  </si>
+  <si>
+    <t>målfokus</t>
+  </si>
+  <si>
+    <t>66959f77-6e2a-4574-8423-3ff097f8b9fa</t>
+  </si>
+  <si>
+    <t>funktionsevneniveau</t>
+  </si>
+  <si>
+    <t>målet udtrykkes i form af et funktionsevneniveau, som kan være et FFB funktionsevneniveau eller FSIII tilstandsniveau</t>
+  </si>
+  <si>
+    <t>90c48f03-f194-4b2f-ad7d-6cba1069ae48</t>
+  </si>
+  <si>
+    <t>måltype</t>
+  </si>
+  <si>
+    <t>målet udtrykkes i form af en måltype, måltypen er den forventede ændring i tilstanden givet indsatsen</t>
   </si>
   <si>
     <t>940f37e6-8a3d-483b-adac-be8af3268a5b</t>
@@ -510,6 +480,15 @@
     <t>udførelse af funktionsevnevurdering i hjemmeplejen jævnfør FSIII</t>
   </si>
   <si>
+    <t>e70c66c0-a939-493b-8ea8-5b7e7b48ba1a</t>
+  </si>
+  <si>
+    <t>generelle oplysninger, FSIII</t>
+  </si>
+  <si>
+    <t>indhentning af generelle oplysninger jævnfør FSIII</t>
+  </si>
+  <si>
     <t>f8ebd11a-04f3-4aa0-9786-406e8896c84d</t>
   </si>
   <si>
@@ -537,15 +516,6 @@
     <t>udførelse af terapeutfaglig udredning jævnfør FSIII</t>
   </si>
   <si>
-    <t>e70c66c0-a939-493b-8ea8-5b7e7b48ba1a</t>
-  </si>
-  <si>
-    <t>generelle oplysninger, FSIII</t>
-  </si>
-  <si>
-    <t>indhentning af generelle oplysninger jævnfør FSIII</t>
-  </si>
-  <si>
     <t>10deb210-e7e1-4d56-9531-b9ff2102126e</t>
   </si>
   <si>
@@ -561,7 +531,10 @@
     <t>4fd6c23a-6ff3-4251-ac37-3ca095027b5b</t>
   </si>
   <si>
-    <t>Det planlagte indsatsforløb vedrører sundhedsfremme og forebyggelse efter §119.</t>
+    <t>Sundhedsfremme og forebyggelse §119</t>
+  </si>
+  <si>
+    <t>Det planlagte indsatsforløb vedrører sundhedsfremme og forebyggelse efter §119</t>
   </si>
   <si>
     <t>5c160c02-e858-4c1f-925a-71ed64844749</t>
@@ -585,7 +558,10 @@
     <t>ddd2f670-5ec7-4f9c-9a2c-aee25cb133bf</t>
   </si>
   <si>
-    <t>Det planlagte indsatsforløb er genoptræning efter sundhedslovens §140.</t>
+    <t>Genoptræning efter §140</t>
+  </si>
+  <si>
+    <t>Det planlagte indsatsforløb er genoptræning efter sundhedslovens §140</t>
   </si>
   <si>
     <t>f15b2663-94d9-4d0c-a5de-d8bd8e1e4ebb</t>
@@ -712,57 +688,6 @@
   </si>
   <si>
     <t>Indsats leveres individuelt</t>
-  </si>
-  <si>
-    <t>bf469e95-f9e3-45c7-bf15-ab7e8a85236f</t>
-  </si>
-  <si>
-    <t>Kontaktklasse</t>
-  </si>
-  <si>
-    <t>Type af kontakt. Beskriver leveringsmetode.</t>
-  </si>
-  <si>
-    <t>1b55a4b0-1156-4f58-b2df-b5c6014d9048</t>
-  </si>
-  <si>
-    <t>Telefonisk</t>
-  </si>
-  <si>
-    <t>Kontakten er foregået per telefon.</t>
-  </si>
-  <si>
-    <t>124be95d-6924-4609-9d2a-e7c73ae3ab3d</t>
-  </si>
-  <si>
-    <t>Skærmbesøg</t>
-  </si>
-  <si>
-    <t>Kontakten er foregået via skærm med mulighed for tændt kamera, så parterne har haft mulighed for at interagere ansigt til ansigt, og fremvise ting.</t>
-  </si>
-  <si>
-    <t>11266a8f-5795-42ab-88ec-4fe5c6c28e80</t>
-  </si>
-  <si>
-    <t>Målfokus</t>
-  </si>
-  <si>
-    <t>66959f77-6e2a-4574-8423-3ff097f8b9fa</t>
-  </si>
-  <si>
-    <t>funktionsevneniveau</t>
-  </si>
-  <si>
-    <t>målet udtrykkes i form af et funktionsevneniveau, som kan være et FFB funktionsevneniveau eller FSIII tilstandsniveau</t>
-  </si>
-  <si>
-    <t>90c48f03-f194-4b2f-ad7d-6cba1069ae48</t>
-  </si>
-  <si>
-    <t>måltype</t>
-  </si>
-  <si>
-    <t>målet udtrykkes i form af en måltype, måltypen er den forventede ændring i tilstanden givet indsatsen</t>
   </si>
 </sst>
 </file>
@@ -1067,7 +992,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D75"/>
+  <dimension ref="A1:D66"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1140,7 +1065,7 @@
         <v>49</v>
       </c>
       <c r="D5" t="s" s="2">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6">
@@ -1148,13 +1073,13 @@
         <v>41</v>
       </c>
       <c r="B6" t="s" s="2">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C6" t="s" s="2">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D6" t="s" s="2">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7">
@@ -1162,10 +1087,10 @@
         <v>41</v>
       </c>
       <c r="B7" t="s" s="2">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C7" t="s" s="2">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D7" t="s" s="2">
         <v>54</v>
@@ -1257,7 +1182,7 @@
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B14" t="s" s="2">
         <v>72</v>
@@ -1271,7 +1196,7 @@
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B15" t="s" s="2">
         <v>75</v>
@@ -1313,30 +1238,30 @@
     </row>
     <row r="18">
       <c r="A18" t="s" s="2">
-        <v>41</v>
+        <v>84</v>
       </c>
       <c r="B18" t="s" s="2">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C18" t="s" s="2">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D18" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="2">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B19" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C19" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D19" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20">
@@ -1344,13 +1269,13 @@
         <v>41</v>
       </c>
       <c r="B20" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C20" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D20" t="s" s="2">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="21">
@@ -1358,13 +1283,13 @@
         <v>41</v>
       </c>
       <c r="B21" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C21" t="s" s="2">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D21" t="s" s="2">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="22">
@@ -1372,13 +1297,13 @@
         <v>41</v>
       </c>
       <c r="B22" t="s" s="2">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C22" t="s" s="2">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D22" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="23">
@@ -1386,18 +1311,18 @@
         <v>41</v>
       </c>
       <c r="B23" t="s" s="2">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C23" t="s" s="2">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D23" t="s" s="2">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="2">
-        <v>102</v>
+        <v>41</v>
       </c>
       <c r="B24" t="s" s="2">
         <v>103</v>
@@ -1411,7 +1336,7 @@
     </row>
     <row r="25">
       <c r="A25" t="s" s="2">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B25" t="s" s="2">
         <v>106</v>
@@ -1439,7 +1364,7 @@
     </row>
     <row r="27">
       <c r="A27" t="s" s="2">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B27" t="s" s="2">
         <v>112</v>
@@ -1448,7 +1373,7 @@
         <v>113</v>
       </c>
       <c r="D27" t="s" s="2">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="28">
@@ -1456,13 +1381,13 @@
         <v>41</v>
       </c>
       <c r="B28" t="s" s="2">
+        <v>114</v>
+      </c>
+      <c r="C28" t="s" s="2">
         <v>115</v>
       </c>
-      <c r="C28" t="s" s="2">
+      <c r="D28" t="s" s="2">
         <v>116</v>
-      </c>
-      <c r="D28" t="s" s="2">
-        <v>117</v>
       </c>
     </row>
     <row r="29">
@@ -1470,27 +1395,27 @@
         <v>41</v>
       </c>
       <c r="B29" t="s" s="2">
+        <v>117</v>
+      </c>
+      <c r="C29" t="s" s="2">
         <v>118</v>
       </c>
-      <c r="C29" t="s" s="2">
+      <c r="D29" t="s" s="2">
         <v>119</v>
-      </c>
-      <c r="D29" t="s" s="2">
-        <v>120</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="2">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B30" t="s" s="2">
+        <v>120</v>
+      </c>
+      <c r="C30" t="s" s="2">
         <v>121</v>
       </c>
-      <c r="C30" t="s" s="2">
-        <v>122</v>
-      </c>
       <c r="D30" t="s" s="2">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="31">
@@ -1498,13 +1423,13 @@
         <v>41</v>
       </c>
       <c r="B31" t="s" s="2">
+        <v>122</v>
+      </c>
+      <c r="C31" t="s" s="2">
+        <v>123</v>
+      </c>
+      <c r="D31" t="s" s="2">
         <v>124</v>
-      </c>
-      <c r="C31" t="s" s="2">
-        <v>125</v>
-      </c>
-      <c r="D31" t="s" s="2">
-        <v>126</v>
       </c>
     </row>
     <row r="32">
@@ -1512,27 +1437,27 @@
         <v>41</v>
       </c>
       <c r="B32" t="s" s="2">
+        <v>125</v>
+      </c>
+      <c r="C32" t="s" s="2">
+        <v>126</v>
+      </c>
+      <c r="D32" t="s" s="2">
         <v>127</v>
-      </c>
-      <c r="C32" t="s" s="2">
-        <v>128</v>
-      </c>
-      <c r="D32" t="s" s="2">
-        <v>129</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="2">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B33" t="s" s="2">
+        <v>128</v>
+      </c>
+      <c r="C33" t="s" s="2">
+        <v>129</v>
+      </c>
+      <c r="D33" t="s" s="2">
         <v>130</v>
-      </c>
-      <c r="C33" t="s" s="2">
-        <v>131</v>
-      </c>
-      <c r="D33" t="s" s="2">
-        <v>131</v>
       </c>
     </row>
     <row r="34">
@@ -1540,13 +1465,13 @@
         <v>41</v>
       </c>
       <c r="B34" t="s" s="2">
+        <v>131</v>
+      </c>
+      <c r="C34" t="s" s="2">
         <v>132</v>
       </c>
-      <c r="C34" t="s" s="2">
-        <v>133</v>
-      </c>
       <c r="D34" t="s" s="2">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="35">
@@ -1554,41 +1479,41 @@
         <v>41</v>
       </c>
       <c r="B35" t="s" s="2">
+        <v>133</v>
+      </c>
+      <c r="C35" t="s" s="2">
+        <v>134</v>
+      </c>
+      <c r="D35" t="s" s="2">
         <v>135</v>
-      </c>
-      <c r="C35" t="s" s="2">
-        <v>136</v>
-      </c>
-      <c r="D35" t="s" s="2">
-        <v>137</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="2">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B36" t="s" s="2">
+        <v>136</v>
+      </c>
+      <c r="C36" t="s" s="2">
+        <v>137</v>
+      </c>
+      <c r="D36" t="s" s="2">
         <v>138</v>
-      </c>
-      <c r="C36" t="s" s="2">
-        <v>139</v>
-      </c>
-      <c r="D36" t="s" s="2">
-        <v>139</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="2">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B37" t="s" s="2">
+        <v>139</v>
+      </c>
+      <c r="C37" t="s" s="2">
         <v>140</v>
       </c>
-      <c r="C37" t="s" s="2">
-        <v>141</v>
-      </c>
       <c r="D37" t="s" s="2">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="38">
@@ -1596,13 +1521,13 @@
         <v>41</v>
       </c>
       <c r="B38" t="s" s="2">
+        <v>141</v>
+      </c>
+      <c r="C38" t="s" s="2">
+        <v>142</v>
+      </c>
+      <c r="D38" t="s" s="2">
         <v>143</v>
-      </c>
-      <c r="C38" t="s" s="2">
-        <v>144</v>
-      </c>
-      <c r="D38" t="s" s="2">
-        <v>145</v>
       </c>
     </row>
     <row r="39">
@@ -1610,27 +1535,27 @@
         <v>41</v>
       </c>
       <c r="B39" t="s" s="2">
+        <v>144</v>
+      </c>
+      <c r="C39" t="s" s="2">
+        <v>145</v>
+      </c>
+      <c r="D39" t="s" s="2">
         <v>146</v>
-      </c>
-      <c r="C39" t="s" s="2">
-        <v>147</v>
-      </c>
-      <c r="D39" t="s" s="2">
-        <v>148</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="2">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B40" t="s" s="2">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C40" t="s" s="2">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D40" t="s" s="2">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="41">
@@ -1638,13 +1563,13 @@
         <v>41</v>
       </c>
       <c r="B41" t="s" s="2">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C41" t="s" s="2">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D41" t="s" s="2">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="42">
@@ -1652,27 +1577,27 @@
         <v>41</v>
       </c>
       <c r="B42" t="s" s="2">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C42" t="s" s="2">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D42" t="s" s="2">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="2">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B43" t="s" s="2">
+        <v>155</v>
+      </c>
+      <c r="C43" t="s" s="2">
+        <v>156</v>
+      </c>
+      <c r="D43" t="s" s="2">
         <v>157</v>
-      </c>
-      <c r="C43" t="s" s="2">
-        <v>158</v>
-      </c>
-      <c r="D43" t="s" s="2">
-        <v>158</v>
       </c>
     </row>
     <row r="44">
@@ -1680,13 +1605,13 @@
         <v>41</v>
       </c>
       <c r="B44" t="s" s="2">
+        <v>158</v>
+      </c>
+      <c r="C44" t="s" s="2">
         <v>159</v>
       </c>
-      <c r="C44" t="s" s="2">
+      <c r="D44" t="s" s="2">
         <v>160</v>
-      </c>
-      <c r="D44" t="s" s="2">
-        <v>161</v>
       </c>
     </row>
     <row r="45">
@@ -1694,13 +1619,13 @@
         <v>41</v>
       </c>
       <c r="B45" t="s" s="2">
+        <v>161</v>
+      </c>
+      <c r="C45" t="s" s="2">
         <v>162</v>
       </c>
-      <c r="C45" t="s" s="2">
+      <c r="D45" t="s" s="2">
         <v>163</v>
-      </c>
-      <c r="D45" t="s" s="2">
-        <v>164</v>
       </c>
     </row>
     <row r="46">
@@ -1708,27 +1633,27 @@
         <v>41</v>
       </c>
       <c r="B46" t="s" s="2">
+        <v>164</v>
+      </c>
+      <c r="C46" t="s" s="2">
         <v>165</v>
       </c>
-      <c r="C46" t="s" s="2">
+      <c r="D46" t="s" s="2">
         <v>166</v>
-      </c>
-      <c r="D46" t="s" s="2">
-        <v>167</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s" s="2">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B47" t="s" s="2">
+        <v>167</v>
+      </c>
+      <c r="C47" t="s" s="2">
         <v>168</v>
       </c>
-      <c r="C47" t="s" s="2">
-        <v>169</v>
-      </c>
       <c r="D47" t="s" s="2">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="48">
@@ -1736,13 +1661,13 @@
         <v>41</v>
       </c>
       <c r="B48" t="s" s="2">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C48" t="s" s="2">
-        <v>172</v>
+        <v>64</v>
       </c>
       <c r="D48" t="s" s="2">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="49">
@@ -1750,41 +1675,41 @@
         <v>41</v>
       </c>
       <c r="B49" t="s" s="2">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C49" t="s" s="2">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D49" t="s" s="2">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s" s="2">
-        <v>38</v>
+        <v>84</v>
       </c>
       <c r="B50" t="s" s="2">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C50" t="s" s="2">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D50" t="s" s="2">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s" s="2">
-        <v>41</v>
+        <v>84</v>
       </c>
       <c r="B51" t="s" s="2">
+        <v>177</v>
+      </c>
+      <c r="C51" t="s" s="2">
+        <v>178</v>
+      </c>
+      <c r="D51" t="s" s="2">
         <v>179</v>
-      </c>
-      <c r="C51" t="s" s="2">
-        <v>58</v>
-      </c>
-      <c r="D51" t="s" s="2">
-        <v>180</v>
       </c>
     </row>
     <row r="52">
@@ -1792,10 +1717,10 @@
         <v>41</v>
       </c>
       <c r="B52" t="s" s="2">
+        <v>180</v>
+      </c>
+      <c r="C52" t="s" s="2">
         <v>181</v>
-      </c>
-      <c r="C52" t="s" s="2">
-        <v>67</v>
       </c>
       <c r="D52" t="s" s="2">
         <v>182</v>
@@ -1803,7 +1728,7 @@
     </row>
     <row r="53">
       <c r="A53" t="s" s="2">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="B53" t="s" s="2">
         <v>183</v>
@@ -1817,7 +1742,7 @@
     </row>
     <row r="54">
       <c r="A54" t="s" s="2">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="B54" t="s" s="2">
         <v>186</v>
@@ -1831,58 +1756,58 @@
     </row>
     <row r="55">
       <c r="A55" t="s" s="2">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B55" t="s" s="2">
         <v>189</v>
       </c>
       <c r="C55" t="s" s="2">
-        <v>70</v>
+        <v>190</v>
       </c>
       <c r="D55" t="s" s="2">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s" s="2">
-        <v>102</v>
+        <v>41</v>
       </c>
       <c r="B56" t="s" s="2">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C56" t="s" s="2">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D56" t="s" s="2">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s" s="2">
-        <v>102</v>
+        <v>41</v>
       </c>
       <c r="B57" t="s" s="2">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C57" t="s" s="2">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D57" t="s" s="2">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s" s="2">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B58" t="s" s="2">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C58" t="s" s="2">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D58" t="s" s="2">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="59">
@@ -1890,237 +1815,111 @@
         <v>41</v>
       </c>
       <c r="B59" t="s" s="2">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C59" t="s" s="2">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D59" t="s" s="2">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s" s="2">
-        <v>41</v>
+        <v>84</v>
       </c>
       <c r="B60" t="s" s="2">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C60" t="s" s="2">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D60" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s" s="2">
-        <v>41</v>
+        <v>84</v>
       </c>
       <c r="B61" t="s" s="2">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C61" t="s" s="2">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D61" t="s" s="2">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s" s="2">
-        <v>41</v>
+        <v>84</v>
       </c>
       <c r="B62" t="s" s="2">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C62" t="s" s="2">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D62" t="s" s="2">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s" s="2">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="B63" t="s" s="2">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C63" t="s" s="2">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D63" t="s" s="2">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s" s="2">
-        <v>102</v>
+        <v>38</v>
       </c>
       <c r="B64" t="s" s="2">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C64" t="s" s="2">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D64" t="s" s="2">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s" s="2">
-        <v>102</v>
+        <v>41</v>
       </c>
       <c r="B65" t="s" s="2">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C65" t="s" s="2">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D65" t="s" s="2">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s" s="2">
-        <v>102</v>
+        <v>41</v>
       </c>
       <c r="B66" t="s" s="2">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C66" t="s" s="2">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="D66" t="s" s="2">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="B67" t="s" s="2">
         <v>224</v>
-      </c>
-      <c r="C67" t="s" s="2">
-        <v>225</v>
-      </c>
-      <c r="D67" t="s" s="2">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="B68" t="s" s="2">
-        <v>227</v>
-      </c>
-      <c r="C68" t="s" s="2">
-        <v>228</v>
-      </c>
-      <c r="D68" t="s" s="2">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="B69" t="s" s="2">
-        <v>230</v>
-      </c>
-      <c r="C69" t="s" s="2">
-        <v>231</v>
-      </c>
-      <c r="D69" t="s" s="2">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="B70" t="s" s="2">
-        <v>233</v>
-      </c>
-      <c r="C70" t="s" s="2">
-        <v>234</v>
-      </c>
-      <c r="D70" t="s" s="2">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="B71" t="s" s="2">
-        <v>236</v>
-      </c>
-      <c r="C71" t="s" s="2">
-        <v>237</v>
-      </c>
-      <c r="D71" t="s" s="2">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="B72" t="s" s="2">
-        <v>239</v>
-      </c>
-      <c r="C72" t="s" s="2">
-        <v>240</v>
-      </c>
-      <c r="D72" t="s" s="2">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="B73" t="s" s="2">
-        <v>242</v>
-      </c>
-      <c r="C73" t="s" s="2">
-        <v>243</v>
-      </c>
-      <c r="D73" t="s" s="2">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="B74" t="s" s="2">
-        <v>244</v>
-      </c>
-      <c r="C74" t="s" s="2">
-        <v>245</v>
-      </c>
-      <c r="D74" t="s" s="2">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="B75" t="s" s="2">
-        <v>247</v>
-      </c>
-      <c r="C75" t="s" s="2">
-        <v>248</v>
-      </c>
-      <c r="D75" t="s" s="2">
-        <v>249</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding term 2.0.0 with four more concepts in FBOE
</commit_message>
<xml_diff>
--- a/term/CodeSystem-CareSocialCodes.xlsx
+++ b/term/CodeSystem-CareSocialCodes.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="250">
   <si>
     <t>Property</t>
   </si>
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>1.1.0</t>
+    <t>2.0.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-07-10T23:08:03+02:00</t>
+    <t>2024-06-04T14:59:10+02:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -69,13 +69,13 @@
     <t>Contact</t>
   </si>
   <si>
-    <t>No display for ContactDetail</t>
+    <t>Kommunernes Landsforening (http://kl.dk)</t>
   </si>
   <si>
     <t>Description</t>
   </si>
   <si>
-    <t>Administrative/technical codes in Local Govenment Denmark (KL), associated with KLCommonCareSocial</t>
+    <t>Administrative/technical codes in Local Govenment Denmark (KL), associated with common use cases across areas or kl-core</t>
   </si>
   <si>
     <t>Purpose</t>
@@ -159,6 +159,18 @@
     <t>Vurdering der sammenholder oplysninger fra udredning mhp en samlet faglig analyse og konklusion.</t>
   </si>
   <si>
+    <t>3f7a8ca0-afca-4b0d-8773-a99b5f2f8aaf</t>
+  </si>
+  <si>
+    <t>VUM Borgerens perspektiv på indsatsen</t>
+  </si>
+  <si>
+    <t>f52887de-023f-4193-b6b0-4b0a37b1cffc</t>
+  </si>
+  <si>
+    <t>VUM Borgerens ressourcer i forhold til indsatsen</t>
+  </si>
+  <si>
     <t>54c4ffea-7caf-4edc-8aa9-ef6e0be26c4c</t>
   </si>
   <si>
@@ -168,67 +180,64 @@
     <t>Sagsvurdering, der sammenholder resultaterne af en myndighedsudredning og den øvrige sagsoplysning med henblik på at træffe en afgørelse</t>
   </si>
   <si>
-    <t>3f7a8ca0-afca-4b0d-8773-a99b5f2f8aaf</t>
-  </si>
-  <si>
-    <t>VUM Borgerens perspektiv på indsatsen</t>
-  </si>
-  <si>
-    <t>f52887de-023f-4193-b6b0-4b0a37b1cffc</t>
-  </si>
-  <si>
-    <t>VUM Borgerens ressourcer i forhold til indsatsen</t>
-  </si>
-  <si>
     <t>7b41185e-eeb4-437d-8120-5d51bbd27a79</t>
   </si>
   <si>
     <t>Indsats/ydelses-anmodning</t>
   </si>
   <si>
+    <t>4a297733-4d66-4726-a933-590d55cf91e0</t>
+  </si>
+  <si>
+    <t>Social indsats</t>
+  </si>
+  <si>
+    <t>Der anmodes om en social indsats</t>
+  </si>
+  <si>
     <t>ad865929-7363-4b2d-a271-01993181fbaf</t>
   </si>
   <si>
-    <t>Hjemmepleje</t>
-  </si>
-  <si>
-    <t>Der anmodes om hjemmepleje</t>
+    <t>Kommunal pleje og omsorg</t>
+  </si>
+  <si>
+    <t>Der anmodes om kommunal pleje og omsorg fx hjemmepleje til ældre borger.</t>
   </si>
   <si>
     <t>490ab7be-ddb1-4a54-baf1-009fe6e8a83b</t>
   </si>
   <si>
-    <t>Hjemmesygepleje</t>
-  </si>
-  <si>
-    <t>Der anmodes om sygepleje</t>
-  </si>
-  <si>
-    <t>4a297733-4d66-4726-a933-590d55cf91e0</t>
-  </si>
-  <si>
-    <t>Social indsats</t>
-  </si>
-  <si>
-    <t>Der anmodes om en social indsats</t>
+    <t>Kommunal sygepleje</t>
+  </si>
+  <si>
+    <t>Der anmodes om kommunal sygepleje.</t>
   </si>
   <si>
     <t>a71921ea-fe83-441d-933b-cc21d0b3c8c3</t>
   </si>
   <si>
-    <t>Sundhedsfremme og forebyggelse</t>
-  </si>
-  <si>
-    <t>Der anmodes om sundhedsfremme og forebyggelse</t>
+    <t>Kommunal Sundhedsfremme og forebyggelse</t>
+  </si>
+  <si>
+    <t>Der anmodes om kommunal sundhedsfremme og forebyggelse efter SUL §119.</t>
   </si>
   <si>
     <t>7fc66c15-0cb3-4c89-9e18-f3a01e6a6592</t>
   </si>
   <si>
-    <t>Træning</t>
-  </si>
-  <si>
-    <t>Der anmodes om træning</t>
+    <t>Kommunal genoptræning efter sygehusophold</t>
+  </si>
+  <si>
+    <t>Der anmodes om kommunal genoptræning efter sygehusophold efter SUL §140.</t>
+  </si>
+  <si>
+    <t>d267ac44-8d7f-43e9-8535-ab3da350649f</t>
+  </si>
+  <si>
+    <t>Kommunalt hjælpemiddelområde</t>
+  </si>
+  <si>
+    <t>Der anmodes om hjælpemidler og lignende, der ligger indenfor det kommunale hjælpemiddelområde dvs § 112, § 113, § 114, § 116 i Serviceloven.</t>
   </si>
   <si>
     <t>b5731132-f6b9-4a47-995d-681d2b755d4f</t>
@@ -258,13 +267,58 @@
     <t>Sagsbehandler er kilde til oplysning eller vurdering</t>
   </si>
   <si>
+    <t>329774f9-7700-47cf-9c00-63765d9e8078</t>
+  </si>
+  <si>
+    <t>Medarbejder og pårørende alene</t>
+  </si>
+  <si>
+    <t>En medarbejder og pårørende er sammen, men uden input fra borger, kilde til oplysning eller vurdering. Fx PUF spørgeskema i sundhedsplejen.</t>
+  </si>
+  <si>
+    <t>8fe80acb-2c2a-4f10-b2b8-ddb77d2f69dc</t>
+  </si>
+  <si>
+    <t>Medarbejder alene</t>
+  </si>
+  <si>
+    <t>Medarbejderen er alene kilde til oplysning eller vurdering. Fx AIMS skema i sundhedsplejen.</t>
+  </si>
+  <si>
+    <t>12428e48-7df8-441f-9a89-d92bb7874066</t>
+  </si>
+  <si>
+    <t>Borger støttet af medarbejder</t>
+  </si>
+  <si>
+    <t>Borger fik hjælp af en medarbejder til at komme med oplysninger eller vurderinger. Fx ældre borger der får hjælp til at udfylde WHO5 spørgeskema.</t>
+  </si>
+  <si>
+    <t>b66dc78a-a673-43fc-8ac0-1e859ba626e0</t>
+  </si>
+  <si>
+    <t>Borger støttet af pårørende</t>
+  </si>
+  <si>
+    <t>Borger fik hjælp af en pårørende til at komme med oplysninger eller vurderinger. Fx ældre borger der får hjælp til at udfylde WHO5 spørgeskema.</t>
+  </si>
+  <si>
+    <t>166d2437-4e47-4a52-bd94-cdbe91086ca6</t>
+  </si>
+  <si>
+    <t>Pårørende alene</t>
+  </si>
+  <si>
+    <t>Pårørende er alene, uden input fra borger, kilde til oplysninger eller vuderderinger. Fx WHO 5 spørgeskema for svækket ældre borger udfyldt af datter.</t>
+  </si>
+  <si>
     <t>63338442-7b2e-405b-acc0-142361ef19f1</t>
   </si>
   <si>
     <t>Andre</t>
   </si>
   <si>
-    <t>Andre end borger og sagsbehandler er kilde til oplysning eller vurdering. Fx læge, pårørende og udfører</t>
+    <t>Andre end borger og sagsbehandler er kilde til oplysning eller vurdering. Fx læge, pårørende og udfører. Denne definition af andre, bruges kun på voksensocialområdet.</t>
   </si>
   <si>
     <t>3</t>
@@ -408,34 +462,289 @@
     <t>Indsatsmål i FFB - er de konkrete faglige mål der arbejdes med, og som er knyttet til tilstande og opfølgninger</t>
   </si>
   <si>
+    <t>ca552020-6ed1-4cdc-b0d4-32697f1f27ad</t>
+  </si>
+  <si>
+    <t>FSIII tilstandsmål</t>
+  </si>
+  <si>
+    <t>Tilstandsmål som defineret af FSIII - ofte i form af en forventet tilstand</t>
+  </si>
+  <si>
+    <t>424827b1-23aa-4848-962b-56ee47def560</t>
+  </si>
+  <si>
+    <t>Indsatsformål</t>
+  </si>
+  <si>
+    <t>Det overordnede formål med hele indsatsen (Defineret af FFB men bruges også for FSIII)</t>
+  </si>
+  <si>
     <t>ffb9886b-d04e-46b1-9165-a400f91f822b</t>
   </si>
   <si>
-    <t>FSIII borgers ønsker og mål</t>
-  </si>
-  <si>
-    <t>ca552020-6ed1-4cdc-b0d4-32697f1f27ad</t>
-  </si>
-  <si>
-    <t>FSIII tilstandsmål</t>
-  </si>
-  <si>
-    <t>Tilstandsmål som defineret af FSIII - ofte i form af en forventet tilstand</t>
-  </si>
-  <si>
-    <t>424827b1-23aa-4848-962b-56ee47def560</t>
-  </si>
-  <si>
-    <t>Indsatsformål</t>
-  </si>
-  <si>
-    <t>Det overordnede formål med hele indsatsen (Defineret af FFB men bruges også for FSIII)</t>
+    <t>Borgers ønsker og mål</t>
+  </si>
+  <si>
+    <t>940f37e6-8a3d-483b-adac-be8af3268a5b</t>
+  </si>
+  <si>
+    <t>oplysningsaktivitet</t>
+  </si>
+  <si>
+    <t>95e787e0-5490-437d-ae4c-f3736644242f</t>
+  </si>
+  <si>
+    <t>afklarende samtale §119, FSIII</t>
+  </si>
+  <si>
+    <t>udførelse af afklarende samtale vedr. sundhedsfremme og forebyggelse jævnfør FSIII</t>
+  </si>
+  <si>
+    <t>e5a73b0e-a5d2-430e-931f-6156306ab00f</t>
+  </si>
+  <si>
+    <t>funktionsevnevurdering hjemmepleje, FSIII</t>
+  </si>
+  <si>
+    <t>udførelse af funktionsevnevurdering i hjemmeplejen jævnfør FSIII</t>
+  </si>
+  <si>
+    <t>f8ebd11a-04f3-4aa0-9786-406e8896c84d</t>
+  </si>
+  <si>
+    <t>socialfaglig udredning, VUM/FFB</t>
+  </si>
+  <si>
+    <t>udførelse af socialfaglig udredning som specificeret af VUM og FFB</t>
+  </si>
+  <si>
+    <t>47fd1468-89da-4803-9d7a-ecc039a30d92</t>
+  </si>
+  <si>
+    <t>sygeplejefaglig udredning, FSIII</t>
+  </si>
+  <si>
+    <t>udførelse af sygeplejefaglig udredning jævnfør FSIII</t>
+  </si>
+  <si>
+    <t>0f0f223c-abe3-4720-aab8-c257679a0a4e</t>
+  </si>
+  <si>
+    <t>terapeutfaglig udredning, FSIII</t>
+  </si>
+  <si>
+    <t>udførelse af terapeutfaglig udredning jævnfør FSIII</t>
+  </si>
+  <si>
+    <t>e70c66c0-a939-493b-8ea8-5b7e7b48ba1a</t>
+  </si>
+  <si>
+    <t>generelle oplysninger, FSIII</t>
+  </si>
+  <si>
+    <t>indhentning af generelle oplysninger jævnfør FSIII</t>
+  </si>
+  <si>
+    <t>10deb210-e7e1-4d56-9531-b9ff2102126e</t>
+  </si>
+  <si>
+    <t>Planlagt indsatsforløb</t>
+  </si>
+  <si>
+    <t>e459386d-1474-4c31-89c5-c8bc7a25e3d4</t>
+  </si>
+  <si>
+    <t>Det planlagte indsatsforløb er en social indsats, som defineret af FFB, med tilhørende ydelser, målgruppe og tilbud</t>
+  </si>
+  <si>
+    <t>4fd6c23a-6ff3-4251-ac37-3ca095027b5b</t>
+  </si>
+  <si>
+    <t>Det planlagte indsatsforløb vedrører sundhedsfremme og forebyggelse efter §119.</t>
+  </si>
+  <si>
+    <t>5c160c02-e858-4c1f-925a-71ed64844749</t>
+  </si>
+  <si>
+    <t>Interventionsforløb efter §119</t>
+  </si>
+  <si>
+    <t>Et planlagt §119 indsatsforløb, som udelukkende indeholder interventioner, og som leveres samlet. Med interventioner menes indsatser, der søger at forbedre borgers tilstand. For §119 kunne et interventionsforløb fx være et KOL-træningshold der indeholder indsatserne fysisk træning og funktionstræning.</t>
+  </si>
+  <si>
+    <t>9791e55a-656f-47eb-8fd5-c4a06b0a4662</t>
+  </si>
+  <si>
+    <t>Opfølgningsforløb efter §119</t>
+  </si>
+  <si>
+    <t>Planlagt indsatsforløb der består af opfølgningsindsatser. Anvendes hvis der i forvejen planlægges opfølgning ved flere forskellige lejligheder fx efter 2,4 og 6 måneder.</t>
+  </si>
+  <si>
+    <t>ddd2f670-5ec7-4f9c-9a2c-aee25cb133bf</t>
+  </si>
+  <si>
+    <t>Det planlagte indsatsforløb er genoptræning efter sundhedslovens §140.</t>
+  </si>
+  <si>
+    <t>f15b2663-94d9-4d0c-a5de-d8bd8e1e4ebb</t>
+  </si>
+  <si>
+    <t>Interventionsforløb efter §140</t>
+  </si>
+  <si>
+    <t>Et planlagt §140 indsatsforløb, som udelukkende indeholder interventioner, og som leveres samlet. Med interventioner menes indsatser, der søger at forbedre borgers tilstand. For §140 kunne et interventionsforløb fx være et Knæ-genoptræningshold der indeholder indsatserne fysisk træning, funktionstræning og vejledning og undervisning.</t>
+  </si>
+  <si>
+    <t>4863001e-14c7-4be8-a2da-e4f21a4b6ac4</t>
+  </si>
+  <si>
+    <t>Opfølgningsforløb efter §140</t>
+  </si>
+  <si>
+    <t>Planlagt indsatsforløb efter §140 der består af opfølgningsindsatser. Anvendes hvis der i forvejen planlægges opfølgning ved flere forskellige lejligheder fx efter 2,4 og 6 måneder.</t>
+  </si>
+  <si>
+    <t>2c059407-fed5-4852-92d8-6bb5ad63d7bb</t>
+  </si>
+  <si>
+    <t>Begrundelse for indsatsophør</t>
+  </si>
+  <si>
+    <t>Begrundelse for, at kommunale indsatser ophører</t>
+  </si>
+  <si>
+    <t>82e99421-31da-4915-96ed-168ccfa1d20c</t>
+  </si>
+  <si>
+    <t>Hændelse medfører ophør</t>
+  </si>
+  <si>
+    <t>Hændelse, som ikke er et aktivt fravalg eller en behovsvurdering medfører ophør. Det kan fx være en længere hospitalsindlæggelse, eller at borger flytter.</t>
+  </si>
+  <si>
+    <t>4bbf6d6a-a1c6-41c2-b8c1-7352b7378adf</t>
+  </si>
+  <si>
+    <t>Ikke yderligere behov (borger-vurderet)</t>
+  </si>
+  <si>
+    <t>Borger vurderer, at han/hun ikke har yderligere behov og afslutter derfor før tid</t>
+  </si>
+  <si>
+    <t>a63b6aa6-7d56-4e67-a5b3-d73f6d262af5</t>
+  </si>
+  <si>
+    <t>Ikke yderligere behov (fagperson-vurderet)</t>
+  </si>
+  <si>
+    <t>Fagperson vurderer, at borger ikke har yderligere behov og afslutter derfor før tid</t>
+  </si>
+  <si>
+    <t>3a5a72b7-addf-4857-b80c-04e4246e3072</t>
+  </si>
+  <si>
+    <t>Aktivt fravalg</t>
+  </si>
+  <si>
+    <t>Borger har behov, men har foretaget et aktivt fravalg</t>
+  </si>
+  <si>
+    <t>0cd5734d-b663-47c6-a3da-6b14a937d144</t>
+  </si>
+  <si>
+    <t>Aktivt fravalg pga. anden sygdom</t>
+  </si>
+  <si>
+    <t>Borger har behov, men har foretaget et aktivt fravalg pga. anden sygdom</t>
+  </si>
+  <si>
+    <t>8371b769-4bfb-4ac8-b130-d91c54784a56</t>
+  </si>
+  <si>
+    <t>Aktivt fravalg pga. logistik ifm. transport</t>
+  </si>
+  <si>
+    <t>Borger har behov, men har foretaget et aktivt fravalg pga. den logistiske udfordring det er mht. transport, at nå frem til det sted indsatsen tilbydes</t>
+  </si>
+  <si>
+    <t>a3f2bd01-078b-486e-81be-797d192ad7bd</t>
+  </si>
+  <si>
+    <t>Aktivt fravalg pga. anden træning</t>
+  </si>
+  <si>
+    <t>Borger har behov, men har foretaget et aktivt fravalg fordi han/hun er påbegyndt træning i andet regi fx fitnesscenter</t>
+  </si>
+  <si>
+    <t>f8436c2e-af1c-44fe-939d-473b518dd01d</t>
+  </si>
+  <si>
+    <t>Aktivt fravalg pga. økonomi ifm. transport</t>
+  </si>
+  <si>
+    <t>Borger har behov, men har foretaget et aktivt fravalg pga. den omkostning der er forbundet med transport til det sted indsatsen tilbydes</t>
+  </si>
+  <si>
+    <t>3f79cee2-b148-4f2c-9cbd-387820e74685</t>
+  </si>
+  <si>
+    <t>Leveringstype</t>
+  </si>
+  <si>
+    <t>Om der leveres individuelt eller gruppebaseret</t>
+  </si>
+  <si>
+    <t>2865f123-15a7-4a36-a514-32ea37c400ca</t>
+  </si>
+  <si>
+    <t>Gruppebaseret indsats</t>
+  </si>
+  <si>
+    <t>Indsats leveres i gruppe</t>
+  </si>
+  <si>
+    <t>8d12d74c-17da-47a7-a4fe-e69dbaec0a8c</t>
+  </si>
+  <si>
+    <t>Individuel indsats</t>
+  </si>
+  <si>
+    <t>Indsats leveres individuelt</t>
+  </si>
+  <si>
+    <t>bf469e95-f9e3-45c7-bf15-ab7e8a85236f</t>
+  </si>
+  <si>
+    <t>Kontaktklasse</t>
+  </si>
+  <si>
+    <t>Type af kontakt. Beskriver leveringsmetode.</t>
+  </si>
+  <si>
+    <t>1b55a4b0-1156-4f58-b2df-b5c6014d9048</t>
+  </si>
+  <si>
+    <t>Telefonisk</t>
+  </si>
+  <si>
+    <t>Kontakten er foregået per telefon.</t>
+  </si>
+  <si>
+    <t>124be95d-6924-4609-9d2a-e7c73ae3ab3d</t>
+  </si>
+  <si>
+    <t>Skærmbesøg</t>
+  </si>
+  <si>
+    <t>Kontakten er foregået via skærm med mulighed for tændt kamera, så parterne har haft mulighed for at interagere ansigt til ansigt, og fremvise ting.</t>
   </si>
   <si>
     <t>11266a8f-5795-42ab-88ec-4fe5c6c28e80</t>
   </si>
   <si>
-    <t>målfokus</t>
+    <t>Målfokus</t>
   </si>
   <si>
     <t>66959f77-6e2a-4574-8423-3ff097f8b9fa</t>
@@ -454,240 +763,6 @@
   </si>
   <si>
     <t>målet udtrykkes i form af en måltype, måltypen er den forventede ændring i tilstanden givet indsatsen</t>
-  </si>
-  <si>
-    <t>940f37e6-8a3d-483b-adac-be8af3268a5b</t>
-  </si>
-  <si>
-    <t>oplysningsaktivitet</t>
-  </si>
-  <si>
-    <t>95e787e0-5490-437d-ae4c-f3736644242f</t>
-  </si>
-  <si>
-    <t>afklarende samtale §119, FSIII</t>
-  </si>
-  <si>
-    <t>udførelse af afklarende samtale vedr. sundhedsfremme og forebyggelse jævnfør FSIII</t>
-  </si>
-  <si>
-    <t>e5a73b0e-a5d2-430e-931f-6156306ab00f</t>
-  </si>
-  <si>
-    <t>funktionsevnevurdering hjemmepleje, FSIII</t>
-  </si>
-  <si>
-    <t>udførelse af funktionsevnevurdering i hjemmeplejen jævnfør FSIII</t>
-  </si>
-  <si>
-    <t>e70c66c0-a939-493b-8ea8-5b7e7b48ba1a</t>
-  </si>
-  <si>
-    <t>generelle oplysninger, FSIII</t>
-  </si>
-  <si>
-    <t>indhentning af generelle oplysninger jævnfør FSIII</t>
-  </si>
-  <si>
-    <t>f8ebd11a-04f3-4aa0-9786-406e8896c84d</t>
-  </si>
-  <si>
-    <t>socialfaglig udredning, VUM/FFB</t>
-  </si>
-  <si>
-    <t>udførelse af socialfaglig udredning som specificeret af VUM og FFB</t>
-  </si>
-  <si>
-    <t>47fd1468-89da-4803-9d7a-ecc039a30d92</t>
-  </si>
-  <si>
-    <t>sygeplejefaglig udredning, FSIII</t>
-  </si>
-  <si>
-    <t>udførelse af sygeplejefaglig udredning jævnfør FSIII</t>
-  </si>
-  <si>
-    <t>0f0f223c-abe3-4720-aab8-c257679a0a4e</t>
-  </si>
-  <si>
-    <t>terapeutfaglig udredning, FSIII</t>
-  </si>
-  <si>
-    <t>udførelse af terapeutfaglig udredning jævnfør FSIII</t>
-  </si>
-  <si>
-    <t>10deb210-e7e1-4d56-9531-b9ff2102126e</t>
-  </si>
-  <si>
-    <t>Planlagt indsatsforløb</t>
-  </si>
-  <si>
-    <t>e459386d-1474-4c31-89c5-c8bc7a25e3d4</t>
-  </si>
-  <si>
-    <t>Det planlagte indsatsforløb er en social indsats, som defineret af FFB, med tilhørende ydelser, målgruppe og tilbud</t>
-  </si>
-  <si>
-    <t>4fd6c23a-6ff3-4251-ac37-3ca095027b5b</t>
-  </si>
-  <si>
-    <t>Sundhedsfremme og forebyggelse §119</t>
-  </si>
-  <si>
-    <t>Det planlagte indsatsforløb vedrører sundhedsfremme og forebyggelse efter §119</t>
-  </si>
-  <si>
-    <t>5c160c02-e858-4c1f-925a-71ed64844749</t>
-  </si>
-  <si>
-    <t>Interventionsforløb efter §119</t>
-  </si>
-  <si>
-    <t>Et planlagt §119 indsatsforløb, som udelukkende indeholder interventioner, og som leveres samlet. Med interventioner menes indsatser, der søger at forbedre borgers tilstand. For §119 kunne et interventionsforløb fx være et KOL-træningshold der indeholder indsatserne fysisk træning og funktionstræning.</t>
-  </si>
-  <si>
-    <t>9791e55a-656f-47eb-8fd5-c4a06b0a4662</t>
-  </si>
-  <si>
-    <t>Opfølgningsforløb efter §119</t>
-  </si>
-  <si>
-    <t>Planlagt indsatsforløb der består af opfølgningsindsatser. Anvendes hvis der i forvejen planlægges opfølgning ved flere forskellige lejligheder fx efter 2,4 og 6 måneder.</t>
-  </si>
-  <si>
-    <t>ddd2f670-5ec7-4f9c-9a2c-aee25cb133bf</t>
-  </si>
-  <si>
-    <t>Genoptræning efter §140</t>
-  </si>
-  <si>
-    <t>Det planlagte indsatsforløb er genoptræning efter sundhedslovens §140</t>
-  </si>
-  <si>
-    <t>f15b2663-94d9-4d0c-a5de-d8bd8e1e4ebb</t>
-  </si>
-  <si>
-    <t>Interventionsforløb efter §140</t>
-  </si>
-  <si>
-    <t>Et planlagt §140 indsatsforløb, som udelukkende indeholder interventioner, og som leveres samlet. Med interventioner menes indsatser, der søger at forbedre borgers tilstand. For §140 kunne et interventionsforløb fx være et Knæ-genoptræningshold der indeholder indsatserne fysisk træning, funktionstræning og vejledning og undervisning.</t>
-  </si>
-  <si>
-    <t>4863001e-14c7-4be8-a2da-e4f21a4b6ac4</t>
-  </si>
-  <si>
-    <t>Opfølgningsforløb efter §140</t>
-  </si>
-  <si>
-    <t>Planlagt indsatsforløb efter §140 der består af opfølgningsindsatser. Anvendes hvis der i forvejen planlægges opfølgning ved flere forskellige lejligheder fx efter 2,4 og 6 måneder.</t>
-  </si>
-  <si>
-    <t>2c059407-fed5-4852-92d8-6bb5ad63d7bb</t>
-  </si>
-  <si>
-    <t>Begrundelse for indsatsophør</t>
-  </si>
-  <si>
-    <t>Begrundelse for, at kommunale indsatser ophører</t>
-  </si>
-  <si>
-    <t>82e99421-31da-4915-96ed-168ccfa1d20c</t>
-  </si>
-  <si>
-    <t>Hændelse medfører ophør</t>
-  </si>
-  <si>
-    <t>Hændelse, som ikke er et aktivt fravalg eller en behovsvurdering medfører ophør. Det kan fx være en længere hospitalsindlæggelse, eller at borger flytter.</t>
-  </si>
-  <si>
-    <t>4bbf6d6a-a1c6-41c2-b8c1-7352b7378adf</t>
-  </si>
-  <si>
-    <t>Ikke yderligere behov (borger-vurderet)</t>
-  </si>
-  <si>
-    <t>Borger vurderer, at han/hun ikke har yderligere behov og afslutter derfor før tid</t>
-  </si>
-  <si>
-    <t>a63b6aa6-7d56-4e67-a5b3-d73f6d262af5</t>
-  </si>
-  <si>
-    <t>Ikke yderligere behov (fagperson-vurderet)</t>
-  </si>
-  <si>
-    <t>Fagperson vurderer, at borger ikke har yderligere behov og afslutter derfor før tid</t>
-  </si>
-  <si>
-    <t>3a5a72b7-addf-4857-b80c-04e4246e3072</t>
-  </si>
-  <si>
-    <t>Aktivt fravalg</t>
-  </si>
-  <si>
-    <t>Borger har behov, men har foretaget et aktivt fravalg</t>
-  </si>
-  <si>
-    <t>0cd5734d-b663-47c6-a3da-6b14a937d144</t>
-  </si>
-  <si>
-    <t>Aktivt fravalg pga. anden sygdom</t>
-  </si>
-  <si>
-    <t>Borger har behov, men har foretaget et aktivt fravalg pga. anden sygdom</t>
-  </si>
-  <si>
-    <t>8371b769-4bfb-4ac8-b130-d91c54784a56</t>
-  </si>
-  <si>
-    <t>Aktivt fravalg pga. logistik ifm. transport</t>
-  </si>
-  <si>
-    <t>Borger har behov, men har foretaget et aktivt fravalg pga. den logistiske udfordring det er mht. transport, at nå frem til det sted indsatsen tilbydes</t>
-  </si>
-  <si>
-    <t>a3f2bd01-078b-486e-81be-797d192ad7bd</t>
-  </si>
-  <si>
-    <t>Aktivt fravalg pga. anden træning</t>
-  </si>
-  <si>
-    <t>Borger har behov, men har foretaget et aktivt fravalg fordi han/hun er påbegyndt træning i andet regi fx fitnesscenter</t>
-  </si>
-  <si>
-    <t>f8436c2e-af1c-44fe-939d-473b518dd01d</t>
-  </si>
-  <si>
-    <t>Aktivt fravalg pga. økonomi ifm. transport</t>
-  </si>
-  <si>
-    <t>Borger har behov, men har foretaget et aktivt fravalg pga. den omkostning der er forbundet med transport til det sted indsatsen tilbydes</t>
-  </si>
-  <si>
-    <t>3f79cee2-b148-4f2c-9cbd-387820e74685</t>
-  </si>
-  <si>
-    <t>Leveringstype</t>
-  </si>
-  <si>
-    <t>Om der leveres individuelt eller gruppebaseret</t>
-  </si>
-  <si>
-    <t>2865f123-15a7-4a36-a514-32ea37c400ca</t>
-  </si>
-  <si>
-    <t>Gruppebaseret indsats</t>
-  </si>
-  <si>
-    <t>Indsats leveres i gruppe</t>
-  </si>
-  <si>
-    <t>8d12d74c-17da-47a7-a4fe-e69dbaec0a8c</t>
-  </si>
-  <si>
-    <t>Individuel indsats</t>
-  </si>
-  <si>
-    <t>Indsats leveres individuelt</t>
   </si>
 </sst>
 </file>
@@ -992,7 +1067,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D66"/>
+  <dimension ref="A1:D75"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1065,7 +1140,7 @@
         <v>49</v>
       </c>
       <c r="D5" t="s" s="2">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6">
@@ -1073,13 +1148,13 @@
         <v>41</v>
       </c>
       <c r="B6" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="C6" t="s" s="2">
         <v>51</v>
       </c>
-      <c r="C6" t="s" s="2">
-        <v>52</v>
-      </c>
       <c r="D6" t="s" s="2">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7">
@@ -1087,10 +1162,10 @@
         <v>41</v>
       </c>
       <c r="B7" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="C7" t="s" s="2">
         <v>53</v>
-      </c>
-      <c r="C7" t="s" s="2">
-        <v>54</v>
       </c>
       <c r="D7" t="s" s="2">
         <v>54</v>
@@ -1182,7 +1257,7 @@
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B14" t="s" s="2">
         <v>72</v>
@@ -1196,7 +1271,7 @@
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B15" t="s" s="2">
         <v>75</v>
@@ -1238,30 +1313,30 @@
     </row>
     <row r="18">
       <c r="A18" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="B18" t="s" s="2">
         <v>84</v>
       </c>
-      <c r="B18" t="s" s="2">
+      <c r="C18" t="s" s="2">
         <v>85</v>
       </c>
-      <c r="C18" t="s" s="2">
+      <c r="D18" t="s" s="2">
         <v>86</v>
-      </c>
-      <c r="D18" t="s" s="2">
-        <v>87</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="2">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B19" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="C19" t="s" s="2">
         <v>88</v>
       </c>
-      <c r="C19" t="s" s="2">
+      <c r="D19" t="s" s="2">
         <v>89</v>
-      </c>
-      <c r="D19" t="s" s="2">
-        <v>90</v>
       </c>
     </row>
     <row r="20">
@@ -1269,13 +1344,13 @@
         <v>41</v>
       </c>
       <c r="B20" t="s" s="2">
+        <v>90</v>
+      </c>
+      <c r="C20" t="s" s="2">
         <v>91</v>
       </c>
-      <c r="C20" t="s" s="2">
+      <c r="D20" t="s" s="2">
         <v>92</v>
-      </c>
-      <c r="D20" t="s" s="2">
-        <v>93</v>
       </c>
     </row>
     <row r="21">
@@ -1283,13 +1358,13 @@
         <v>41</v>
       </c>
       <c r="B21" t="s" s="2">
+        <v>93</v>
+      </c>
+      <c r="C21" t="s" s="2">
         <v>94</v>
       </c>
-      <c r="C21" t="s" s="2">
+      <c r="D21" t="s" s="2">
         <v>95</v>
-      </c>
-      <c r="D21" t="s" s="2">
-        <v>96</v>
       </c>
     </row>
     <row r="22">
@@ -1297,13 +1372,13 @@
         <v>41</v>
       </c>
       <c r="B22" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="C22" t="s" s="2">
         <v>97</v>
       </c>
-      <c r="C22" t="s" s="2">
+      <c r="D22" t="s" s="2">
         <v>98</v>
-      </c>
-      <c r="D22" t="s" s="2">
-        <v>99</v>
       </c>
     </row>
     <row r="23">
@@ -1311,18 +1386,18 @@
         <v>41</v>
       </c>
       <c r="B23" t="s" s="2">
+        <v>99</v>
+      </c>
+      <c r="C23" t="s" s="2">
         <v>100</v>
       </c>
-      <c r="C23" t="s" s="2">
+      <c r="D23" t="s" s="2">
         <v>101</v>
-      </c>
-      <c r="D23" t="s" s="2">
-        <v>102</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="2">
-        <v>41</v>
+        <v>102</v>
       </c>
       <c r="B24" t="s" s="2">
         <v>103</v>
@@ -1336,7 +1411,7 @@
     </row>
     <row r="25">
       <c r="A25" t="s" s="2">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B25" t="s" s="2">
         <v>106</v>
@@ -1364,7 +1439,7 @@
     </row>
     <row r="27">
       <c r="A27" t="s" s="2">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B27" t="s" s="2">
         <v>112</v>
@@ -1373,7 +1448,7 @@
         <v>113</v>
       </c>
       <c r="D27" t="s" s="2">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="28">
@@ -1381,13 +1456,13 @@
         <v>41</v>
       </c>
       <c r="B28" t="s" s="2">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C28" t="s" s="2">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D28" t="s" s="2">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="29">
@@ -1395,27 +1470,27 @@
         <v>41</v>
       </c>
       <c r="B29" t="s" s="2">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C29" t="s" s="2">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D29" t="s" s="2">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="2">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B30" t="s" s="2">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C30" t="s" s="2">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D30" t="s" s="2">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="31">
@@ -1423,13 +1498,13 @@
         <v>41</v>
       </c>
       <c r="B31" t="s" s="2">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C31" t="s" s="2">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D31" t="s" s="2">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="32">
@@ -1437,27 +1512,27 @@
         <v>41</v>
       </c>
       <c r="B32" t="s" s="2">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C32" t="s" s="2">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D32" t="s" s="2">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="2">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B33" t="s" s="2">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C33" t="s" s="2">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="D33" t="s" s="2">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="34">
@@ -1465,13 +1540,13 @@
         <v>41</v>
       </c>
       <c r="B34" t="s" s="2">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C34" t="s" s="2">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D34" t="s" s="2">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="35">
@@ -1479,41 +1554,41 @@
         <v>41</v>
       </c>
       <c r="B35" t="s" s="2">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C35" t="s" s="2">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="D35" t="s" s="2">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="2">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B36" t="s" s="2">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C36" t="s" s="2">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D36" t="s" s="2">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="2">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B37" t="s" s="2">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C37" t="s" s="2">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D37" t="s" s="2">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="38">
@@ -1521,13 +1596,13 @@
         <v>41</v>
       </c>
       <c r="B38" t="s" s="2">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C38" t="s" s="2">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D38" t="s" s="2">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="39">
@@ -1535,27 +1610,27 @@
         <v>41</v>
       </c>
       <c r="B39" t="s" s="2">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C39" t="s" s="2">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D39" t="s" s="2">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="2">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B40" t="s" s="2">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="C40" t="s" s="2">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D40" t="s" s="2">
-        <v>148</v>
+        <v>151</v>
       </c>
     </row>
     <row r="41">
@@ -1563,13 +1638,13 @@
         <v>41</v>
       </c>
       <c r="B41" t="s" s="2">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="C41" t="s" s="2">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="D41" t="s" s="2">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
     <row r="42">
@@ -1577,27 +1652,27 @@
         <v>41</v>
       </c>
       <c r="B42" t="s" s="2">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="C42" t="s" s="2">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="D42" t="s" s="2">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="2">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B43" t="s" s="2">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C43" t="s" s="2">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D43" t="s" s="2">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="44">
@@ -1605,13 +1680,13 @@
         <v>41</v>
       </c>
       <c r="B44" t="s" s="2">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C44" t="s" s="2">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D44" t="s" s="2">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="45">
@@ -1619,13 +1694,13 @@
         <v>41</v>
       </c>
       <c r="B45" t="s" s="2">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C45" t="s" s="2">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D45" t="s" s="2">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="46">
@@ -1633,27 +1708,27 @@
         <v>41</v>
       </c>
       <c r="B46" t="s" s="2">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C46" t="s" s="2">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D46" t="s" s="2">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s" s="2">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B47" t="s" s="2">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C47" t="s" s="2">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D47" t="s" s="2">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="48">
@@ -1661,13 +1736,13 @@
         <v>41</v>
       </c>
       <c r="B48" t="s" s="2">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="C48" t="s" s="2">
-        <v>64</v>
+        <v>172</v>
       </c>
       <c r="D48" t="s" s="2">
-        <v>170</v>
+        <v>173</v>
       </c>
     </row>
     <row r="49">
@@ -1675,41 +1750,41 @@
         <v>41</v>
       </c>
       <c r="B49" t="s" s="2">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="C49" t="s" s="2">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="D49" t="s" s="2">
-        <v>173</v>
+        <v>176</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s" s="2">
-        <v>84</v>
+        <v>38</v>
       </c>
       <c r="B50" t="s" s="2">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="C50" t="s" s="2">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="D50" t="s" s="2">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s" s="2">
-        <v>84</v>
+        <v>41</v>
       </c>
       <c r="B51" t="s" s="2">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C51" t="s" s="2">
-        <v>178</v>
+        <v>58</v>
       </c>
       <c r="D51" t="s" s="2">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="52">
@@ -1717,10 +1792,10 @@
         <v>41</v>
       </c>
       <c r="B52" t="s" s="2">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C52" t="s" s="2">
-        <v>181</v>
+        <v>67</v>
       </c>
       <c r="D52" t="s" s="2">
         <v>182</v>
@@ -1728,7 +1803,7 @@
     </row>
     <row r="53">
       <c r="A53" t="s" s="2">
-        <v>84</v>
+        <v>102</v>
       </c>
       <c r="B53" t="s" s="2">
         <v>183</v>
@@ -1742,7 +1817,7 @@
     </row>
     <row r="54">
       <c r="A54" t="s" s="2">
-        <v>84</v>
+        <v>102</v>
       </c>
       <c r="B54" t="s" s="2">
         <v>186</v>
@@ -1756,58 +1831,58 @@
     </row>
     <row r="55">
       <c r="A55" t="s" s="2">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B55" t="s" s="2">
         <v>189</v>
       </c>
       <c r="C55" t="s" s="2">
+        <v>70</v>
+      </c>
+      <c r="D55" t="s" s="2">
         <v>190</v>
-      </c>
-      <c r="D55" t="s" s="2">
-        <v>191</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s" s="2">
-        <v>41</v>
+        <v>102</v>
       </c>
       <c r="B56" t="s" s="2">
+        <v>191</v>
+      </c>
+      <c r="C56" t="s" s="2">
         <v>192</v>
       </c>
-      <c r="C56" t="s" s="2">
+      <c r="D56" t="s" s="2">
         <v>193</v>
-      </c>
-      <c r="D56" t="s" s="2">
-        <v>194</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s" s="2">
-        <v>41</v>
+        <v>102</v>
       </c>
       <c r="B57" t="s" s="2">
+        <v>194</v>
+      </c>
+      <c r="C57" t="s" s="2">
         <v>195</v>
       </c>
-      <c r="C57" t="s" s="2">
+      <c r="D57" t="s" s="2">
         <v>196</v>
-      </c>
-      <c r="D57" t="s" s="2">
-        <v>197</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s" s="2">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B58" t="s" s="2">
+        <v>197</v>
+      </c>
+      <c r="C58" t="s" s="2">
         <v>198</v>
       </c>
-      <c r="C58" t="s" s="2">
+      <c r="D58" t="s" s="2">
         <v>199</v>
-      </c>
-      <c r="D58" t="s" s="2">
-        <v>200</v>
       </c>
     </row>
     <row r="59">
@@ -1815,111 +1890,237 @@
         <v>41</v>
       </c>
       <c r="B59" t="s" s="2">
+        <v>200</v>
+      </c>
+      <c r="C59" t="s" s="2">
         <v>201</v>
       </c>
-      <c r="C59" t="s" s="2">
+      <c r="D59" t="s" s="2">
         <v>202</v>
-      </c>
-      <c r="D59" t="s" s="2">
-        <v>203</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s" s="2">
-        <v>84</v>
+        <v>41</v>
       </c>
       <c r="B60" t="s" s="2">
+        <v>203</v>
+      </c>
+      <c r="C60" t="s" s="2">
         <v>204</v>
       </c>
-      <c r="C60" t="s" s="2">
+      <c r="D60" t="s" s="2">
         <v>205</v>
-      </c>
-      <c r="D60" t="s" s="2">
-        <v>206</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s" s="2">
-        <v>84</v>
+        <v>41</v>
       </c>
       <c r="B61" t="s" s="2">
+        <v>206</v>
+      </c>
+      <c r="C61" t="s" s="2">
         <v>207</v>
       </c>
-      <c r="C61" t="s" s="2">
+      <c r="D61" t="s" s="2">
         <v>208</v>
-      </c>
-      <c r="D61" t="s" s="2">
-        <v>209</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s" s="2">
-        <v>84</v>
+        <v>41</v>
       </c>
       <c r="B62" t="s" s="2">
+        <v>209</v>
+      </c>
+      <c r="C62" t="s" s="2">
         <v>210</v>
       </c>
-      <c r="C62" t="s" s="2">
+      <c r="D62" t="s" s="2">
         <v>211</v>
-      </c>
-      <c r="D62" t="s" s="2">
-        <v>212</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s" s="2">
-        <v>84</v>
+        <v>102</v>
       </c>
       <c r="B63" t="s" s="2">
+        <v>212</v>
+      </c>
+      <c r="C63" t="s" s="2">
         <v>213</v>
       </c>
-      <c r="C63" t="s" s="2">
+      <c r="D63" t="s" s="2">
         <v>214</v>
-      </c>
-      <c r="D63" t="s" s="2">
-        <v>215</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s" s="2">
-        <v>38</v>
+        <v>102</v>
       </c>
       <c r="B64" t="s" s="2">
+        <v>215</v>
+      </c>
+      <c r="C64" t="s" s="2">
         <v>216</v>
       </c>
-      <c r="C64" t="s" s="2">
+      <c r="D64" t="s" s="2">
         <v>217</v>
-      </c>
-      <c r="D64" t="s" s="2">
-        <v>218</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s" s="2">
-        <v>41</v>
+        <v>102</v>
       </c>
       <c r="B65" t="s" s="2">
+        <v>218</v>
+      </c>
+      <c r="C65" t="s" s="2">
         <v>219</v>
       </c>
-      <c r="C65" t="s" s="2">
+      <c r="D65" t="s" s="2">
         <v>220</v>
-      </c>
-      <c r="D65" t="s" s="2">
-        <v>221</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s" s="2">
-        <v>41</v>
+        <v>102</v>
       </c>
       <c r="B66" t="s" s="2">
+        <v>221</v>
+      </c>
+      <c r="C66" t="s" s="2">
         <v>222</v>
       </c>
-      <c r="C66" t="s" s="2">
+      <c r="D66" t="s" s="2">
         <v>223</v>
       </c>
-      <c r="D66" t="s" s="2">
+    </row>
+    <row r="67">
+      <c r="A67" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="B67" t="s" s="2">
         <v>224</v>
+      </c>
+      <c r="C67" t="s" s="2">
+        <v>225</v>
+      </c>
+      <c r="D67" t="s" s="2">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="B68" t="s" s="2">
+        <v>227</v>
+      </c>
+      <c r="C68" t="s" s="2">
+        <v>228</v>
+      </c>
+      <c r="D68" t="s" s="2">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="B69" t="s" s="2">
+        <v>230</v>
+      </c>
+      <c r="C69" t="s" s="2">
+        <v>231</v>
+      </c>
+      <c r="D69" t="s" s="2">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="B70" t="s" s="2">
+        <v>233</v>
+      </c>
+      <c r="C70" t="s" s="2">
+        <v>234</v>
+      </c>
+      <c r="D70" t="s" s="2">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="B71" t="s" s="2">
+        <v>236</v>
+      </c>
+      <c r="C71" t="s" s="2">
+        <v>237</v>
+      </c>
+      <c r="D71" t="s" s="2">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="B72" t="s" s="2">
+        <v>239</v>
+      </c>
+      <c r="C72" t="s" s="2">
+        <v>240</v>
+      </c>
+      <c r="D72" t="s" s="2">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="B73" t="s" s="2">
+        <v>242</v>
+      </c>
+      <c r="C73" t="s" s="2">
+        <v>243</v>
+      </c>
+      <c r="D73" t="s" s="2">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="B74" t="s" s="2">
+        <v>244</v>
+      </c>
+      <c r="C74" t="s" s="2">
+        <v>245</v>
+      </c>
+      <c r="D74" t="s" s="2">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="B75" t="s" s="2">
+        <v>247</v>
+      </c>
+      <c r="C75" t="s" s="2">
+        <v>248</v>
+      </c>
+      <c r="D75" t="s" s="2">
+        <v>249</v>
       </c>
     </row>
   </sheetData>

</xml_diff>